<commit_message>
Atualizacao tesouro 21/05 -  Criacao titulo liliane - atualizacao livio
</commit_message>
<xml_diff>
--- a/TITULO COMPRADO - LIVIO.xlsx
+++ b/TITULO COMPRADO - LIVIO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="020519" sheetId="1" r:id="rId1"/>
-    <sheet name="PLANILHAS" sheetId="2" r:id="rId2"/>
+    <sheet name="GRAFICO" sheetId="2" r:id="rId2"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId3"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="18">
   <si>
     <t>DATA COMPRA</t>
   </si>
@@ -81,7 +81,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="8" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00"/>
-    <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="dd/mm"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
@@ -151,7 +151,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -280,12 +280,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -332,12 +355,6 @@
     </xf>
     <xf numFmtId="8" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -413,9 +430,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="3" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Moeda" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -513,15 +542,15 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:idx val="2"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>PLANILHAS!$A$4</c:f>
+              <c:f>GRAFICO!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>VENDA</c:v>
+                  <c:v>TITULO VENDA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -529,7 +558,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent3"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -540,11 +569,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent3"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent3"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -555,13 +584,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PLANILHAS!$B$2:$AC$3</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$2:$AE$3</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(PLANILHAS!$D$2:$D$3,PLANILHAS!$F$2:$F$3,PLANILHAS!$H$2:$H$3,PLANILHAS!$J$2:$J$3,PLANILHAS!$L$2:$L$3,PLANILHAS!$N$2:$N$3,PLANILHAS!$P$2:$P$3,PLANILHAS!$R$2:$R$3,PLANILHAS!$T$2:$T$3,PLANILHAS!$V$2:$V$3,PLANILHAS!$X$2:$X$3,PLANILHAS!$Z$2:$Z$3,PLANILHAS!$AB$2:$AB$3)</c:f>
+              <c:f>(GRAFICO!$D$2:$D$3,GRAFICO!$F$2:$F$3,GRAFICO!$H$2:$H$3,GRAFICO!$J$2:$J$3,GRAFICO!$L$2:$L$3,GRAFICO!$N$2:$N$3,GRAFICO!$P$2:$P$3,GRAFICO!$R$2:$R$3,GRAFICO!$T$2:$T$3,GRAFICO!$V$2:$V$3,GRAFICO!$X$2:$X$3,GRAFICO!$Z$2:$Z$3,GRAFICO!$AB$2:$AB$3,GRAFICO!$AD$2:$AD$3)</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>02/05</c:v>
@@ -601,6 +630,9 @@
                   </c:pt>
                   <c:pt idx="12">
                     <c:v>20/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>21/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -641,6 +673,9 @@
                     <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="12">
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
                     <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                 </c:lvl>
@@ -652,52 +687,55 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PLANILHAS!$B$4:$AC$4</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$6:$AE$6</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(PLANILHAS!$D$4,PLANILHAS!$F$4,PLANILHAS!$H$4,PLANILHAS!$J$4,PLANILHAS!$L$4,PLANILHAS!$N$4,PLANILHAS!$P$4,PLANILHAS!$R$4,PLANILHAS!$T$4,PLANILHAS!$V$4,PLANILHAS!$X$4,PLANILHAS!$Z$4,PLANILHAS!$AB$4)</c:f>
+              <c:f>(GRAFICO!$D$6,GRAFICO!$F$6,GRAFICO!$H$6,GRAFICO!$J$6,GRAFICO!$L$6,GRAFICO!$N$6,GRAFICO!$P$6,GRAFICO!$R$6,GRAFICO!$T$6,GRAFICO!$V$6,GRAFICO!$X$6,GRAFICO!$Z$6,GRAFICO!$AB$6,GRAFICO!$AD$6)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>4.5599999999999996</c:v>
-                </c:pt>
-                <c:pt idx="1" formatCode="General">
-                  <c:v>4.54</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="General">
-                  <c:v>4.5199999999999996</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="General">
-                  <c:v>4.5</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="General">
-                  <c:v>4.49</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="General">
-                  <c:v>4.49</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="General">
-                  <c:v>4.4400000000000004</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="General">
-                  <c:v>4.42</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="General">
-                  <c:v>4.46</c:v>
-                </c:pt>
-                <c:pt idx="9" formatCode="General">
-                  <c:v>4.42</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="General">
-                  <c:v>4.42</c:v>
-                </c:pt>
-                <c:pt idx="11" formatCode="General">
-                  <c:v>4.4400000000000004</c:v>
-                </c:pt>
-                <c:pt idx="12" formatCode="General">
-                  <c:v>4.47</c:v>
+                <c:ptCount val="14"/>
+                <c:pt idx="0" formatCode="0.00">
+                  <c:v>0.25463106728435353</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="0.00">
+                  <c:v>0.25365530303030304</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.00">
+                  <c:v>0.25278396436525613</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00">
+                  <c:v>0.251917012031876</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00">
+                  <c:v>0.25143776166010628</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00">
+                  <c:v>0.25134338815316193</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.00">
+                  <c:v>0.24932826142265854</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.00">
+                  <c:v>0.24847712753786311</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.00">
+                  <c:v>0.24990981128789483</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.00">
+                  <c:v>0.24832202321355731</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="0.00">
+                  <c:v>0.2482560474528098</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="0.00">
+                  <c:v>0.24890196685767385</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="0.00">
+                  <c:v>0.24997822435139677</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="0.00">
+                  <c:v>0.24313922457352755</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -705,15 +743,15 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:idx val="3"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>PLANILHAS!$A$5</c:f>
+              <c:f>GRAFICO!$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>COMPRA</c:v>
+                  <c:v>TITULO COMPRA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -721,7 +759,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent4"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -732,11 +770,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent4"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent2"/>
+                  <a:schemeClr val="accent4"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -747,13 +785,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PLANILHAS!$B$2:$AC$3</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$2:$AE$3</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(PLANILHAS!$D$2:$D$3,PLANILHAS!$F$2:$F$3,PLANILHAS!$H$2:$H$3,PLANILHAS!$J$2:$J$3,PLANILHAS!$L$2:$L$3,PLANILHAS!$N$2:$N$3,PLANILHAS!$P$2:$P$3,PLANILHAS!$R$2:$R$3,PLANILHAS!$T$2:$T$3,PLANILHAS!$V$2:$V$3,PLANILHAS!$X$2:$X$3,PLANILHAS!$Z$2:$Z$3,PLANILHAS!$AB$2:$AB$3)</c:f>
+              <c:f>(GRAFICO!$D$2:$D$3,GRAFICO!$F$2:$F$3,GRAFICO!$H$2:$H$3,GRAFICO!$J$2:$J$3,GRAFICO!$L$2:$L$3,GRAFICO!$N$2:$N$3,GRAFICO!$P$2:$P$3,GRAFICO!$R$2:$R$3,GRAFICO!$T$2:$T$3,GRAFICO!$V$2:$V$3,GRAFICO!$X$2:$X$3,GRAFICO!$Z$2:$Z$3,GRAFICO!$AB$2:$AB$3,GRAFICO!$AD$2:$AD$3)</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>02/05</c:v>
@@ -793,6 +831,9 @@
                   </c:pt>
                   <c:pt idx="12">
                     <c:v>20/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>21/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -833,6 +874,9 @@
                     <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="12">
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
                     <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                 </c:lvl>
@@ -844,52 +888,55 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PLANILHAS!$B$5:$AC$5</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$7:$AE$7</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(PLANILHAS!$D$5,PLANILHAS!$F$5,PLANILHAS!$H$5,PLANILHAS!$J$5,PLANILHAS!$L$5,PLANILHAS!$N$5,PLANILHAS!$P$5,PLANILHAS!$R$5,PLANILHAS!$T$5,PLANILHAS!$V$5,PLANILHAS!$X$5,PLANILHAS!$Z$5,PLANILHAS!$AB$5)</c:f>
+              <c:f>(GRAFICO!$D$7,GRAFICO!$F$7,GRAFICO!$H$7,GRAFICO!$J$7,GRAFICO!$L$7,GRAFICO!$N$7,GRAFICO!$P$7,GRAFICO!$R$7,GRAFICO!$T$7,GRAFICO!$V$7,GRAFICO!$X$7,GRAFICO!$Z$7,GRAFICO!$AB$7,GRAFICO!$AD$7)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>4.4400000000000004</c:v>
-                </c:pt>
-                <c:pt idx="1" formatCode="General">
-                  <c:v>4.42</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="General">
-                  <c:v>4.4000000000000004</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="General">
-                  <c:v>4.38</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="General">
-                  <c:v>4.37</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="General">
-                  <c:v>4.37</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="General">
-                  <c:v>4.32</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="General">
-                  <c:v>4.3</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="General">
-                  <c:v>4.34</c:v>
-                </c:pt>
-                <c:pt idx="9" formatCode="General">
-                  <c:v>4.3</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="General">
-                  <c:v>4.3</c:v>
-                </c:pt>
-                <c:pt idx="11" formatCode="General">
-                  <c:v>4.32</c:v>
-                </c:pt>
-                <c:pt idx="12" formatCode="General">
-                  <c:v>4.3499999999999996</c:v>
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="0.00">
+                  <c:v>0.24904081569405279</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.00">
+                  <c:v>0.248187040583112</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00">
+                  <c:v>0.24733605422076124</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00">
+                  <c:v>0.24686647496866476</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00">
+                  <c:v>0.24677398551748281</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.00">
+                  <c:v>0.24479388792084519</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.00">
+                  <c:v>0.24396004736027202</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.00">
+                  <c:v>0.2453694373706099</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.00">
+                  <c:v>0.24380904992202529</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="0.00">
+                  <c:v>0.24374545013346274</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="0.00">
+                  <c:v>0.24438294507633357</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="0.00">
+                  <c:v>0.24544138398665863</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="0.00">
+                  <c:v>0.24763483738158781</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -906,11 +953,441 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="579911488"/>
-        <c:axId val="579905504"/>
+        <c:axId val="1206586400"/>
+        <c:axId val="1206590752"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>GRAFICO!$A$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>VENDA</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:cat>
+                  <c:multiLvlStrRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>GRAFICO!$B$2:$AE$3</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>(GRAFICO!$D$2:$D$3,GRAFICO!$F$2:$F$3,GRAFICO!$H$2:$H$3,GRAFICO!$J$2:$J$3,GRAFICO!$L$2:$L$3,GRAFICO!$N$2:$N$3,GRAFICO!$P$2:$P$3,GRAFICO!$R$2:$R$3,GRAFICO!$T$2:$T$3,GRAFICO!$V$2:$V$3,GRAFICO!$X$2:$X$3,GRAFICO!$Z$2:$Z$3,GRAFICO!$AB$2:$AB$3,GRAFICO!$AD$2:$AD$3)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:multiLvlStrCache>
+                      <c:ptCount val="14"/>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>02/05</c:v>
+                        </c:pt>
+                        <c:pt idx="1">
+                          <c:v>03/05</c:v>
+                        </c:pt>
+                        <c:pt idx="2">
+                          <c:v>06/05</c:v>
+                        </c:pt>
+                        <c:pt idx="3">
+                          <c:v>07/05</c:v>
+                        </c:pt>
+                        <c:pt idx="4">
+                          <c:v>08/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="5">
+                          <c:v>09/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="6">
+                          <c:v>10/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="7">
+                          <c:v>13/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="8">
+                          <c:v>14/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="9">
+                          <c:v>15/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="10">
+                          <c:v>16/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="11">
+                          <c:v>17/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="12">
+                          <c:v>20/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="13">
+                          <c:v>21/mai</c:v>
+                        </c:pt>
+                      </c:lvl>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="1">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="2">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="3">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="4">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="5">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="6">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="7">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="8">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="9">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="10">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="11">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="12">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="13">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                      </c:lvl>
+                    </c:multiLvlStrCache>
+                  </c:multiLvlStrRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>GRAFICO!$B$4:$AE$4</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>(GRAFICO!$D$4,GRAFICO!$F$4,GRAFICO!$H$4,GRAFICO!$J$4,GRAFICO!$L$4,GRAFICO!$N$4,GRAFICO!$P$4,GRAFICO!$R$4,GRAFICO!$T$4,GRAFICO!$V$4,GRAFICO!$X$4,GRAFICO!$Z$4,GRAFICO!$AB$4,GRAFICO!$AD$4)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>m/d/yyyy</c:formatCode>
+                      <c:ptCount val="14"/>
+                      <c:pt idx="0" formatCode="General">
+                        <c:v>4.5599999999999996</c:v>
+                      </c:pt>
+                      <c:pt idx="1" formatCode="General">
+                        <c:v>4.54</c:v>
+                      </c:pt>
+                      <c:pt idx="2" formatCode="General">
+                        <c:v>4.5199999999999996</c:v>
+                      </c:pt>
+                      <c:pt idx="3" formatCode="General">
+                        <c:v>4.5</c:v>
+                      </c:pt>
+                      <c:pt idx="4" formatCode="General">
+                        <c:v>4.49</c:v>
+                      </c:pt>
+                      <c:pt idx="5" formatCode="General">
+                        <c:v>4.49</c:v>
+                      </c:pt>
+                      <c:pt idx="6" formatCode="General">
+                        <c:v>4.4400000000000004</c:v>
+                      </c:pt>
+                      <c:pt idx="7" formatCode="General">
+                        <c:v>4.42</c:v>
+                      </c:pt>
+                      <c:pt idx="8" formatCode="General">
+                        <c:v>4.46</c:v>
+                      </c:pt>
+                      <c:pt idx="9" formatCode="General">
+                        <c:v>4.42</c:v>
+                      </c:pt>
+                      <c:pt idx="10" formatCode="General">
+                        <c:v>4.42</c:v>
+                      </c:pt>
+                      <c:pt idx="11" formatCode="General">
+                        <c:v>4.4400000000000004</c:v>
+                      </c:pt>
+                      <c:pt idx="12" formatCode="General">
+                        <c:v>4.47</c:v>
+                      </c:pt>
+                      <c:pt idx="13" formatCode="General">
+                        <c:v>4.29</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>GRAFICO!$A$5</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>COMPRA</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:cat>
+                  <c:multiLvlStrRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>GRAFICO!$B$2:$AE$3</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>(GRAFICO!$D$2:$D$3,GRAFICO!$F$2:$F$3,GRAFICO!$H$2:$H$3,GRAFICO!$J$2:$J$3,GRAFICO!$L$2:$L$3,GRAFICO!$N$2:$N$3,GRAFICO!$P$2:$P$3,GRAFICO!$R$2:$R$3,GRAFICO!$T$2:$T$3,GRAFICO!$V$2:$V$3,GRAFICO!$X$2:$X$3,GRAFICO!$Z$2:$Z$3,GRAFICO!$AB$2:$AB$3,GRAFICO!$AD$2:$AD$3)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:multiLvlStrCache>
+                      <c:ptCount val="14"/>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>02/05</c:v>
+                        </c:pt>
+                        <c:pt idx="1">
+                          <c:v>03/05</c:v>
+                        </c:pt>
+                        <c:pt idx="2">
+                          <c:v>06/05</c:v>
+                        </c:pt>
+                        <c:pt idx="3">
+                          <c:v>07/05</c:v>
+                        </c:pt>
+                        <c:pt idx="4">
+                          <c:v>08/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="5">
+                          <c:v>09/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="6">
+                          <c:v>10/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="7">
+                          <c:v>13/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="8">
+                          <c:v>14/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="9">
+                          <c:v>15/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="10">
+                          <c:v>16/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="11">
+                          <c:v>17/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="12">
+                          <c:v>20/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="13">
+                          <c:v>21/mai</c:v>
+                        </c:pt>
+                      </c:lvl>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="1">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="2">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="3">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="4">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="5">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="6">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="7">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="8">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="9">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="10">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="11">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="12">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="13">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                      </c:lvl>
+                    </c:multiLvlStrCache>
+                  </c:multiLvlStrRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>GRAFICO!$B$5:$AE$5</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>(GRAFICO!$D$5,GRAFICO!$F$5,GRAFICO!$H$5,GRAFICO!$J$5,GRAFICO!$L$5,GRAFICO!$N$5,GRAFICO!$P$5,GRAFICO!$R$5,GRAFICO!$T$5,GRAFICO!$V$5,GRAFICO!$X$5,GRAFICO!$Z$5,GRAFICO!$AB$5,GRAFICO!$AD$5)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>m/d/yyyy</c:formatCode>
+                      <c:ptCount val="14"/>
+                      <c:pt idx="0" formatCode="General">
+                        <c:v>4.4400000000000004</c:v>
+                      </c:pt>
+                      <c:pt idx="1" formatCode="General">
+                        <c:v>4.42</c:v>
+                      </c:pt>
+                      <c:pt idx="2" formatCode="General">
+                        <c:v>4.4000000000000004</c:v>
+                      </c:pt>
+                      <c:pt idx="3" formatCode="General">
+                        <c:v>4.38</c:v>
+                      </c:pt>
+                      <c:pt idx="4" formatCode="General">
+                        <c:v>4.37</c:v>
+                      </c:pt>
+                      <c:pt idx="5" formatCode="General">
+                        <c:v>4.37</c:v>
+                      </c:pt>
+                      <c:pt idx="6" formatCode="General">
+                        <c:v>4.32</c:v>
+                      </c:pt>
+                      <c:pt idx="7" formatCode="General">
+                        <c:v>4.3</c:v>
+                      </c:pt>
+                      <c:pt idx="8" formatCode="General">
+                        <c:v>4.34</c:v>
+                      </c:pt>
+                      <c:pt idx="9" formatCode="General">
+                        <c:v>4.3</c:v>
+                      </c:pt>
+                      <c:pt idx="10" formatCode="General">
+                        <c:v>4.3</c:v>
+                      </c:pt>
+                      <c:pt idx="11" formatCode="General">
+                        <c:v>4.32</c:v>
+                      </c:pt>
+                      <c:pt idx="12" formatCode="General">
+                        <c:v>4.3499999999999996</c:v>
+                      </c:pt>
+                      <c:pt idx="13" formatCode="General">
+                        <c:v>4.41</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="579911488"/>
+        <c:axId val="1206586400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -953,7 +1430,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="579905504"/>
+        <c:crossAx val="1206590752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -961,7 +1438,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="579905504"/>
+        <c:axId val="1206590752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -981,7 +1458,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="&quot;R$&quot;#,##0.00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1012,7 +1489,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="579911488"/>
+        <c:crossAx val="1206586400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1179,7 +1656,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>PLANILHAS!$A$4</c:f>
+              <c:f>GRAFICO!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1217,11 +1694,11 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PLANILHAS!$B$2:$AC$3</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$2:$AC$3</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(PLANILHAS!$E$2:$E$3,PLANILHAS!$G$2:$G$3,PLANILHAS!$I$2:$I$3,PLANILHAS!$K$2:$K$3,PLANILHAS!$M$2:$M$3,PLANILHAS!$O$2:$O$3,PLANILHAS!$Q$2:$Q$3,PLANILHAS!$S$2:$S$3,PLANILHAS!$U$2:$U$3,PLANILHAS!$W$2:$W$3,PLANILHAS!$Y$2:$Y$3,PLANILHAS!$AA$2:$AA$3,PLANILHAS!$AC$2:$AC$3)</c:f>
+              <c:f>(GRAFICO!$E$2:$E$3,GRAFICO!$G$2:$G$3,GRAFICO!$I$2:$I$3,GRAFICO!$K$2:$K$3,GRAFICO!$M$2:$M$3,GRAFICO!$O$2:$O$3,GRAFICO!$Q$2:$Q$3,GRAFICO!$S$2:$S$3,GRAFICO!$U$2:$U$3,GRAFICO!$W$2:$W$3,GRAFICO!$Y$2:$Y$3,GRAFICO!$AA$2:$AA$3,GRAFICO!$AC$2:$AC$3)</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="13"/>
                 <c:lvl>
@@ -1314,11 +1791,11 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PLANILHAS!$B$4:$AC$4</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$4:$AC$4</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(PLANILHAS!$E$4,PLANILHAS!$G$4,PLANILHAS!$I$4,PLANILHAS!$K$4,PLANILHAS!$M$4,PLANILHAS!$O$4,PLANILHAS!$Q$4,PLANILHAS!$S$4,PLANILHAS!$U$4,PLANILHAS!$W$4,PLANILHAS!$Y$4,PLANILHAS!$AA$4,PLANILHAS!$AC$4)</c:f>
+              <c:f>(GRAFICO!$E$4,GRAFICO!$G$4,GRAFICO!$I$4,GRAFICO!$K$4,GRAFICO!$M$4,GRAFICO!$O$4,GRAFICO!$Q$4,GRAFICO!$S$4,GRAFICO!$U$4,GRAFICO!$W$4,GRAFICO!$Y$4,GRAFICO!$AA$4,GRAFICO!$AC$4)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1371,7 +1848,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>PLANILHAS!$A$5</c:f>
+              <c:f>GRAFICO!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1409,11 +1886,11 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PLANILHAS!$B$2:$AC$3</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$2:$AC$3</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(PLANILHAS!$E$2:$E$3,PLANILHAS!$G$2:$G$3,PLANILHAS!$I$2:$I$3,PLANILHAS!$K$2:$K$3,PLANILHAS!$M$2:$M$3,PLANILHAS!$O$2:$O$3,PLANILHAS!$Q$2:$Q$3,PLANILHAS!$S$2:$S$3,PLANILHAS!$U$2:$U$3,PLANILHAS!$W$2:$W$3,PLANILHAS!$Y$2:$Y$3,PLANILHAS!$AA$2:$AA$3,PLANILHAS!$AC$2:$AC$3)</c:f>
+              <c:f>(GRAFICO!$E$2:$E$3,GRAFICO!$G$2:$G$3,GRAFICO!$I$2:$I$3,GRAFICO!$K$2:$K$3,GRAFICO!$M$2:$M$3,GRAFICO!$O$2:$O$3,GRAFICO!$Q$2:$Q$3,GRAFICO!$S$2:$S$3,GRAFICO!$U$2:$U$3,GRAFICO!$W$2:$W$3,GRAFICO!$Y$2:$Y$3,GRAFICO!$AA$2:$AA$3,GRAFICO!$AC$2:$AC$3)</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="13"/>
                 <c:lvl>
@@ -1506,11 +1983,11 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PLANILHAS!$B$5:$AC$5</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$5:$AC$5</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(PLANILHAS!$E$5,PLANILHAS!$G$5,PLANILHAS!$I$5,PLANILHAS!$K$5,PLANILHAS!$M$5,PLANILHAS!$O$5,PLANILHAS!$Q$5,PLANILHAS!$S$5,PLANILHAS!$U$5,PLANILHAS!$W$5,PLANILHAS!$Y$5,PLANILHAS!$AA$5,PLANILHAS!$AC$5)</c:f>
+              <c:f>(GRAFICO!$E$5,GRAFICO!$G$5,GRAFICO!$I$5,GRAFICO!$K$5,GRAFICO!$M$5,GRAFICO!$O$5,GRAFICO!$Q$5,GRAFICO!$S$5,GRAFICO!$U$5,GRAFICO!$W$5,GRAFICO!$Y$5,GRAFICO!$AA$5,GRAFICO!$AC$5)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1568,11 +2045,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="579909856"/>
-        <c:axId val="579910944"/>
+        <c:axId val="1206588576"/>
+        <c:axId val="1206589120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="579909856"/>
+        <c:axId val="1206588576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1615,7 +2092,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="579910944"/>
+        <c:crossAx val="1206589120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1623,7 +2100,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="579910944"/>
+        <c:axId val="1206589120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1674,7 +2151,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="579909856"/>
+        <c:crossAx val="1206588576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1811,7 +2288,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>PLANILHAS!$A$6</c:f>
+              <c:f>GRAFICO!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1849,13 +2326,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PLANILHAS!$B$2:$AC$3</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$2:$AE$3</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(PLANILHAS!$D$2:$D$3,PLANILHAS!$F$2:$F$3,PLANILHAS!$H$2:$H$3,PLANILHAS!$J$2:$J$3,PLANILHAS!$L$2:$L$3,PLANILHAS!$N$2:$N$3,PLANILHAS!$P$2:$P$3,PLANILHAS!$R$2:$R$3,PLANILHAS!$T$2:$T$3,PLANILHAS!$V$2:$V$3,PLANILHAS!$X$2:$X$3,PLANILHAS!$Z$2:$Z$3,PLANILHAS!$AB$2:$AB$3)</c:f>
+              <c:f>(GRAFICO!$E$2:$E$3,GRAFICO!$G$2:$G$3,GRAFICO!$I$2:$I$3,GRAFICO!$K$2:$K$3,GRAFICO!$M$2:$M$3,GRAFICO!$O$2:$O$3,GRAFICO!$Q$2:$Q$3,GRAFICO!$S$2:$S$3,GRAFICO!$U$2:$U$3,GRAFICO!$W$2:$W$3,GRAFICO!$Y$2:$Y$3,GRAFICO!$AA$2:$AA$3,GRAFICO!$AC$2:$AC$3,GRAFICO!$AE$2:$AE$3)</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>02/05</c:v>
@@ -1896,46 +2373,52 @@
                   <c:pt idx="12">
                     <c:v>20/mai</c:v>
                   </c:pt>
+                  <c:pt idx="13">
+                    <c:v>21/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                    <c:v>Preço Unitário</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                    <c:v>Preço Unitário</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                    <c:v>Preço Unitário</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                    <c:v>Preço Unitário</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                    <c:v>Preço Unitário</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                    <c:v>Preço Unitário</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                    <c:v>Preço Unitário</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                    <c:v>Preço Unitário</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                    <c:v>Preço Unitário</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                    <c:v>Preço Unitário</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                    <c:v>Preço Unitário</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                    <c:v>Preço Unitário</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                    <c:v>Preço Unitário</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>Preço Unitário</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -1946,52 +2429,55 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PLANILHAS!$B$6:$AC$6</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$6:$AE$6</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(PLANILHAS!$D$6,PLANILHAS!$F$6,PLANILHAS!$H$6,PLANILHAS!$J$6,PLANILHAS!$L$6,PLANILHAS!$N$6,PLANILHAS!$P$6,PLANILHAS!$R$6,PLANILHAS!$T$6,PLANILHAS!$V$6,PLANILHAS!$X$6,PLANILHAS!$Z$6,PLANILHAS!$AB$6)</c:f>
+              <c:f>(GRAFICO!$E$6,GRAFICO!$G$6,GRAFICO!$I$6,GRAFICO!$K$6,GRAFICO!$M$6,GRAFICO!$O$6,GRAFICO!$Q$6,GRAFICO!$S$6,GRAFICO!$U$6,GRAFICO!$W$6,GRAFICO!$Y$6,GRAFICO!$AA$6,GRAFICO!$AC$6,GRAFICO!$AE$6)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:ptCount val="14"/>
+                <c:pt idx="0" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                   <c:v>5.01962301369863</c:v>
                 </c:pt>
-                <c:pt idx="1" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="1" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                   <c:v>4.9976071232876711</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="2" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                   <c:v>4.9755912328767122</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="3" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                   <c:v>4.9535753424657534</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="4" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                   <c:v>4.9425673972602748</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="5" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                   <c:v>4.9425673972602748</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="6" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                   <c:v>4.8875276712328777</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="7" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                   <c:v>4.8655117808219179</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="8" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                   <c:v>4.9095435616438357</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="9" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                   <c:v>4.8655117808219179</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="10" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                   <c:v>4.8655117808219179</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="11" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                   <c:v>4.8875276712328777</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="12" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                   <c:v>4.9205515068493151</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>4.7224084931506853</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2003,7 +2489,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>PLANILHAS!$A$7</c:f>
+              <c:f>GRAFICO!$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2041,13 +2527,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PLANILHAS!$B$2:$AC$3</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$2:$AE$3</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(PLANILHAS!$D$2:$D$3,PLANILHAS!$F$2:$F$3,PLANILHAS!$H$2:$H$3,PLANILHAS!$J$2:$J$3,PLANILHAS!$L$2:$L$3,PLANILHAS!$N$2:$N$3,PLANILHAS!$P$2:$P$3,PLANILHAS!$R$2:$R$3,PLANILHAS!$T$2:$T$3,PLANILHAS!$V$2:$V$3,PLANILHAS!$X$2:$X$3,PLANILHAS!$Z$2:$Z$3,PLANILHAS!$AB$2:$AB$3)</c:f>
+              <c:f>(GRAFICO!$E$2:$E$3,GRAFICO!$G$2:$G$3,GRAFICO!$I$2:$I$3,GRAFICO!$K$2:$K$3,GRAFICO!$M$2:$M$3,GRAFICO!$O$2:$O$3,GRAFICO!$Q$2:$Q$3,GRAFICO!$S$2:$S$3,GRAFICO!$U$2:$U$3,GRAFICO!$W$2:$W$3,GRAFICO!$Y$2:$Y$3,GRAFICO!$AA$2:$AA$3,GRAFICO!$AC$2:$AC$3,GRAFICO!$AE$2:$AE$3)</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>02/05</c:v>
@@ -2088,46 +2574,52 @@
                   <c:pt idx="12">
                     <c:v>20/mai</c:v>
                   </c:pt>
+                  <c:pt idx="13">
+                    <c:v>21/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                    <c:v>Preço Unitário</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                    <c:v>Preço Unitário</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                    <c:v>Preço Unitário</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                    <c:v>Preço Unitário</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                    <c:v>Preço Unitário</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                    <c:v>Preço Unitário</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                    <c:v>Preço Unitário</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                    <c:v>Preço Unitário</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                    <c:v>Preço Unitário</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                    <c:v>Preço Unitário</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                    <c:v>Preço Unitário</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                    <c:v>Preço Unitário</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                    <c:v>Preço Unitário</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>Preço Unitário</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -2138,52 +2630,55 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PLANILHAS!$B$7:$AC$7</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$7:$AE$7</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(PLANILHAS!$D$7,PLANILHAS!$F$7,PLANILHAS!$H$7,PLANILHAS!$J$7,PLANILHAS!$L$7,PLANILHAS!$N$7,PLANILHAS!$P$7,PLANILHAS!$R$7,PLANILHAS!$T$7,PLANILHAS!$V$7,PLANILHAS!$X$7,PLANILHAS!$Z$7,PLANILHAS!$AB$7)</c:f>
+              <c:f>(GRAFICO!$E$7,GRAFICO!$G$7,GRAFICO!$I$7,GRAFICO!$K$7,GRAFICO!$M$7,GRAFICO!$O$7,GRAFICO!$Q$7,GRAFICO!$S$7,GRAFICO!$U$7,GRAFICO!$W$7,GRAFICO!$Y$7,GRAFICO!$AA$7,GRAFICO!$AC$7,GRAFICO!$AE$7)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:ptCount val="14"/>
+                <c:pt idx="0" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                   <c:v>4.8875276712328777</c:v>
                 </c:pt>
-                <c:pt idx="1" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="1" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                   <c:v>4.8655117808219179</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="2" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                   <c:v>4.8434958904109591</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="3" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                   <c:v>4.8214800000000002</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="4" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                   <c:v>4.8104720547945208</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="5" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                   <c:v>4.8104720547945208</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="6" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                   <c:v>4.7554323287671245</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="7" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                   <c:v>4.7334164383561648</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="8" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                   <c:v>4.7774482191780825</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="9" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                   <c:v>4.7334164383561648</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="10" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                   <c:v>4.7334164383561648</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="11" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                   <c:v>4.7554323287671245</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                <c:pt idx="12" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                   <c:v>4.788456164383561</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>4.8545038356164385</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2200,8 +2695,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="652648272"/>
-        <c:axId val="652638480"/>
+        <c:axId val="1206590208"/>
+        <c:axId val="1206591296"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -2213,7 +2708,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>PLANILHAS!$A$4</c15:sqref>
+                          <c15:sqref>GRAFICO!$A$4</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -2254,15 +2749,15 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>PLANILHAS!$B$2:$AC$3</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$2:$AE$3</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(PLANILHAS!$D$2:$D$3,PLANILHAS!$F$2:$F$3,PLANILHAS!$H$2:$H$3,PLANILHAS!$J$2:$J$3,PLANILHAS!$L$2:$L$3,PLANILHAS!$N$2:$N$3,PLANILHAS!$P$2:$P$3,PLANILHAS!$R$2:$R$3,PLANILHAS!$T$2:$T$3,PLANILHAS!$V$2:$V$3,PLANILHAS!$X$2:$X$3,PLANILHAS!$Z$2:$Z$3,PLANILHAS!$AB$2:$AB$3)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$E$2:$E$3,GRAFICO!$G$2:$G$3,GRAFICO!$I$2:$I$3,GRAFICO!$K$2:$K$3,GRAFICO!$M$2:$M$3,GRAFICO!$O$2:$O$3,GRAFICO!$Q$2:$Q$3,GRAFICO!$S$2:$S$3,GRAFICO!$U$2:$U$3,GRAFICO!$W$2:$W$3,GRAFICO!$Y$2:$Y$3,GRAFICO!$AA$2:$AA$3,GRAFICO!$AC$2:$AC$3,GRAFICO!$AE$2:$AE$3)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:multiLvlStrCache>
-                      <c:ptCount val="13"/>
+                      <c:ptCount val="14"/>
                       <c:lvl>
                         <c:pt idx="0">
                           <c:v>02/05</c:v>
@@ -2303,46 +2798,52 @@
                         <c:pt idx="12">
                           <c:v>20/mai</c:v>
                         </c:pt>
+                        <c:pt idx="13">
+                          <c:v>21/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
-                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                          <c:v>Preço Unitário</c:v>
                         </c:pt>
                         <c:pt idx="1">
-                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                          <c:v>Preço Unitário</c:v>
                         </c:pt>
                         <c:pt idx="2">
-                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                          <c:v>Preço Unitário</c:v>
                         </c:pt>
                         <c:pt idx="3">
-                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                          <c:v>Preço Unitário</c:v>
                         </c:pt>
                         <c:pt idx="4">
-                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                          <c:v>Preço Unitário</c:v>
                         </c:pt>
                         <c:pt idx="5">
-                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                          <c:v>Preço Unitário</c:v>
                         </c:pt>
                         <c:pt idx="6">
-                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                          <c:v>Preço Unitário</c:v>
                         </c:pt>
                         <c:pt idx="7">
-                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                          <c:v>Preço Unitário</c:v>
                         </c:pt>
                         <c:pt idx="8">
-                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                          <c:v>Preço Unitário</c:v>
                         </c:pt>
                         <c:pt idx="9">
-                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                          <c:v>Preço Unitário</c:v>
                         </c:pt>
                         <c:pt idx="10">
-                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                          <c:v>Preço Unitário</c:v>
                         </c:pt>
                         <c:pt idx="11">
-                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                          <c:v>Preço Unitário</c:v>
                         </c:pt>
                         <c:pt idx="12">
-                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                          <c:v>Preço Unitário</c:v>
+                        </c:pt>
+                        <c:pt idx="13">
+                          <c:v>Preço Unitário</c:v>
                         </c:pt>
                       </c:lvl>
                     </c:multiLvlStrCache>
@@ -2353,54 +2854,57 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>PLANILHAS!$B$4:$AC$4</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$4:$AE$4</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(PLANILHAS!$D$4,PLANILHAS!$F$4,PLANILHAS!$H$4,PLANILHAS!$J$4,PLANILHAS!$L$4,PLANILHAS!$N$4,PLANILHAS!$P$4,PLANILHAS!$R$4,PLANILHAS!$T$4,PLANILHAS!$V$4,PLANILHAS!$X$4,PLANILHAS!$Z$4,PLANILHAS!$AB$4)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$E$4,GRAFICO!$G$4,GRAFICO!$I$4,GRAFICO!$K$4,GRAFICO!$M$4,GRAFICO!$O$4,GRAFICO!$Q$4,GRAFICO!$S$4,GRAFICO!$U$4,GRAFICO!$W$4,GRAFICO!$Y$4,GRAFICO!$AA$4,GRAFICO!$AC$4,GRAFICO!$AE$4)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>m/d/yyyy</c:formatCode>
-                      <c:ptCount val="13"/>
-                      <c:pt idx="0" formatCode="General">
-                        <c:v>4.5599999999999996</c:v>
-                      </c:pt>
-                      <c:pt idx="1" formatCode="General">
-                        <c:v>4.54</c:v>
-                      </c:pt>
-                      <c:pt idx="2" formatCode="General">
-                        <c:v>4.5199999999999996</c:v>
-                      </c:pt>
-                      <c:pt idx="3" formatCode="General">
-                        <c:v>4.5</c:v>
-                      </c:pt>
-                      <c:pt idx="4" formatCode="General">
-                        <c:v>4.49</c:v>
-                      </c:pt>
-                      <c:pt idx="5" formatCode="General">
-                        <c:v>4.49</c:v>
-                      </c:pt>
-                      <c:pt idx="6" formatCode="General">
-                        <c:v>4.4400000000000004</c:v>
-                      </c:pt>
-                      <c:pt idx="7" formatCode="General">
-                        <c:v>4.42</c:v>
-                      </c:pt>
-                      <c:pt idx="8" formatCode="General">
-                        <c:v>4.46</c:v>
-                      </c:pt>
-                      <c:pt idx="9" formatCode="General">
-                        <c:v>4.42</c:v>
-                      </c:pt>
-                      <c:pt idx="10" formatCode="General">
-                        <c:v>4.42</c:v>
-                      </c:pt>
-                      <c:pt idx="11" formatCode="General">
-                        <c:v>4.4400000000000004</c:v>
-                      </c:pt>
-                      <c:pt idx="12" formatCode="General">
-                        <c:v>4.47</c:v>
+                      <c:ptCount val="14"/>
+                      <c:pt idx="0" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1577.93</c:v>
+                      </c:pt>
+                      <c:pt idx="1" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1584</c:v>
+                      </c:pt>
+                      <c:pt idx="2" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1589.46</c:v>
+                      </c:pt>
+                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1594.93</c:v>
+                      </c:pt>
+                      <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1597.97</c:v>
+                      </c:pt>
+                      <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1598.57</c:v>
+                      </c:pt>
+                      <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1611.49</c:v>
+                      </c:pt>
+                      <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1617.01</c:v>
+                      </c:pt>
+                      <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1607.74</c:v>
+                      </c:pt>
+                      <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1618.02</c:v>
+                      </c:pt>
+                      <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1618.45</c:v>
+                      </c:pt>
+                      <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1614.25</c:v>
+                      </c:pt>
+                      <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1607.3</c:v>
+                      </c:pt>
+                      <c:pt idx="13" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1652.51</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2417,7 +2921,7 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>PLANILHAS!$A$5</c15:sqref>
+                          <c15:sqref>GRAFICO!$A$5</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -2458,15 +2962,15 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>PLANILHAS!$B$2:$AC$3</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$2:$AE$3</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(PLANILHAS!$D$2:$D$3,PLANILHAS!$F$2:$F$3,PLANILHAS!$H$2:$H$3,PLANILHAS!$J$2:$J$3,PLANILHAS!$L$2:$L$3,PLANILHAS!$N$2:$N$3,PLANILHAS!$P$2:$P$3,PLANILHAS!$R$2:$R$3,PLANILHAS!$T$2:$T$3,PLANILHAS!$V$2:$V$3,PLANILHAS!$X$2:$X$3,PLANILHAS!$Z$2:$Z$3,PLANILHAS!$AB$2:$AB$3)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$E$2:$E$3,GRAFICO!$G$2:$G$3,GRAFICO!$I$2:$I$3,GRAFICO!$K$2:$K$3,GRAFICO!$M$2:$M$3,GRAFICO!$O$2:$O$3,GRAFICO!$Q$2:$Q$3,GRAFICO!$S$2:$S$3,GRAFICO!$U$2:$U$3,GRAFICO!$W$2:$W$3,GRAFICO!$Y$2:$Y$3,GRAFICO!$AA$2:$AA$3,GRAFICO!$AC$2:$AC$3,GRAFICO!$AE$2:$AE$3)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:multiLvlStrCache>
-                      <c:ptCount val="13"/>
+                      <c:ptCount val="14"/>
                       <c:lvl>
                         <c:pt idx="0">
                           <c:v>02/05</c:v>
@@ -2507,46 +3011,52 @@
                         <c:pt idx="12">
                           <c:v>20/mai</c:v>
                         </c:pt>
+                        <c:pt idx="13">
+                          <c:v>21/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
-                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                          <c:v>Preço Unitário</c:v>
                         </c:pt>
                         <c:pt idx="1">
-                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                          <c:v>Preço Unitário</c:v>
                         </c:pt>
                         <c:pt idx="2">
-                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                          <c:v>Preço Unitário</c:v>
                         </c:pt>
                         <c:pt idx="3">
-                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                          <c:v>Preço Unitário</c:v>
                         </c:pt>
                         <c:pt idx="4">
-                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                          <c:v>Preço Unitário</c:v>
                         </c:pt>
                         <c:pt idx="5">
-                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                          <c:v>Preço Unitário</c:v>
                         </c:pt>
                         <c:pt idx="6">
-                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                          <c:v>Preço Unitário</c:v>
                         </c:pt>
                         <c:pt idx="7">
-                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                          <c:v>Preço Unitário</c:v>
                         </c:pt>
                         <c:pt idx="8">
-                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                          <c:v>Preço Unitário</c:v>
                         </c:pt>
                         <c:pt idx="9">
-                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                          <c:v>Preço Unitário</c:v>
                         </c:pt>
                         <c:pt idx="10">
-                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                          <c:v>Preço Unitário</c:v>
                         </c:pt>
                         <c:pt idx="11">
-                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                          <c:v>Preço Unitário</c:v>
                         </c:pt>
                         <c:pt idx="12">
-                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                          <c:v>Preço Unitário</c:v>
+                        </c:pt>
+                        <c:pt idx="13">
+                          <c:v>Preço Unitário</c:v>
                         </c:pt>
                       </c:lvl>
                     </c:multiLvlStrCache>
@@ -2557,54 +3067,57 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>PLANILHAS!$B$5:$AC$5</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$5:$AE$5</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(PLANILHAS!$D$5,PLANILHAS!$F$5,PLANILHAS!$H$5,PLANILHAS!$J$5,PLANILHAS!$L$5,PLANILHAS!$N$5,PLANILHAS!$P$5,PLANILHAS!$R$5,PLANILHAS!$T$5,PLANILHAS!$V$5,PLANILHAS!$X$5,PLANILHAS!$Z$5,PLANILHAS!$AB$5)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$E$5,GRAFICO!$G$5,GRAFICO!$I$5,GRAFICO!$K$5,GRAFICO!$M$5,GRAFICO!$O$5,GRAFICO!$Q$5,GRAFICO!$S$5,GRAFICO!$U$5,GRAFICO!$W$5,GRAFICO!$Y$5,GRAFICO!$AA$5,GRAFICO!$AC$5,GRAFICO!$AE$5)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>m/d/yyyy</c:formatCode>
-                      <c:ptCount val="13"/>
-                      <c:pt idx="0" formatCode="General">
-                        <c:v>4.4400000000000004</c:v>
-                      </c:pt>
-                      <c:pt idx="1" formatCode="General">
-                        <c:v>4.42</c:v>
-                      </c:pt>
-                      <c:pt idx="2" formatCode="General">
-                        <c:v>4.4000000000000004</c:v>
-                      </c:pt>
-                      <c:pt idx="3" formatCode="General">
-                        <c:v>4.38</c:v>
-                      </c:pt>
-                      <c:pt idx="4" formatCode="General">
-                        <c:v>4.37</c:v>
-                      </c:pt>
-                      <c:pt idx="5" formatCode="General">
-                        <c:v>4.37</c:v>
-                      </c:pt>
-                      <c:pt idx="6" formatCode="General">
-                        <c:v>4.32</c:v>
-                      </c:pt>
-                      <c:pt idx="7" formatCode="General">
-                        <c:v>4.3</c:v>
-                      </c:pt>
-                      <c:pt idx="8" formatCode="General">
-                        <c:v>4.34</c:v>
-                      </c:pt>
-                      <c:pt idx="9" formatCode="General">
-                        <c:v>4.3</c:v>
-                      </c:pt>
-                      <c:pt idx="10" formatCode="General">
-                        <c:v>4.3</c:v>
-                      </c:pt>
-                      <c:pt idx="11" formatCode="General">
-                        <c:v>4.32</c:v>
-                      </c:pt>
-                      <c:pt idx="12" formatCode="General">
-                        <c:v>4.3499999999999996</c:v>
+                      <c:ptCount val="14"/>
+                      <c:pt idx="0" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1607.16</c:v>
+                      </c:pt>
+                      <c:pt idx="1" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1613.35</c:v>
+                      </c:pt>
+                      <c:pt idx="2" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1618.9</c:v>
+                      </c:pt>
+                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1624.47</c:v>
+                      </c:pt>
+                      <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1627.56</c:v>
+                      </c:pt>
+                      <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1628.17</c:v>
+                      </c:pt>
+                      <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1641.34</c:v>
+                      </c:pt>
+                      <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1646.95</c:v>
+                      </c:pt>
+                      <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1637.49</c:v>
+                      </c:pt>
+                      <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1647.97</c:v>
+                      </c:pt>
+                      <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1648.4</c:v>
+                      </c:pt>
+                      <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1644.1</c:v>
+                      </c:pt>
+                      <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1637.01</c:v>
+                      </c:pt>
+                      <c:pt idx="13" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1622.51</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2616,7 +3129,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="652648272"/>
+        <c:axId val="1206590208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2659,7 +3172,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="652638480"/>
+        <c:crossAx val="1206591296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2667,7 +3180,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="652638480"/>
+        <c:axId val="1206591296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2687,7 +3200,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2718,7 +3231,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="652648272"/>
+        <c:crossAx val="1206590208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2855,7 +3368,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>PLANILHAS!$A$6</c:f>
+              <c:f>GRAFICO!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2893,11 +3406,11 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PLANILHAS!$B$2:$AC$3</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$2:$AC$3</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(PLANILHAS!$E$2:$E$3,PLANILHAS!$G$2:$G$3,PLANILHAS!$I$2:$I$3,PLANILHAS!$K$2:$K$3,PLANILHAS!$M$2:$M$3,PLANILHAS!$O$2:$O$3,PLANILHAS!$Q$2:$Q$3,PLANILHAS!$S$2:$S$3,PLANILHAS!$U$2:$U$3,PLANILHAS!$W$2:$W$3,PLANILHAS!$Y$2:$Y$3,PLANILHAS!$AA$2:$AA$3,PLANILHAS!$AC$2:$AC$3)</c:f>
+              <c:f>(GRAFICO!$E$2:$E$3,GRAFICO!$G$2:$G$3,GRAFICO!$I$2:$I$3,GRAFICO!$K$2:$K$3,GRAFICO!$M$2:$M$3,GRAFICO!$O$2:$O$3,GRAFICO!$Q$2:$Q$3,GRAFICO!$S$2:$S$3,GRAFICO!$U$2:$U$3,GRAFICO!$W$2:$W$3,GRAFICO!$Y$2:$Y$3,GRAFICO!$AA$2:$AA$3,GRAFICO!$AC$2:$AC$3)</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="13"/>
                 <c:lvl>
@@ -2990,52 +3503,52 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PLANILHAS!$B$6:$AC$6</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$6:$AC$6</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(PLANILHAS!$E$6,PLANILHAS!$G$6,PLANILHAS!$I$6,PLANILHAS!$K$6,PLANILHAS!$M$6,PLANILHAS!$O$6,PLANILHAS!$Q$6,PLANILHAS!$S$6,PLANILHAS!$U$6,PLANILHAS!$W$6,PLANILHAS!$Y$6,PLANILHAS!$AA$6,PLANILHAS!$AC$6)</c:f>
+              <c:f>(GRAFICO!$E$6,GRAFICO!$G$6,GRAFICO!$I$6,GRAFICO!$K$6,GRAFICO!$M$6,GRAFICO!$O$6,GRAFICO!$Q$6,GRAFICO!$S$6,GRAFICO!$U$6,GRAFICO!$W$6,GRAFICO!$Y$6,GRAFICO!$AA$6,GRAFICO!$AC$6)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="13"/>
-                <c:pt idx="0" formatCode="0.00">
-                  <c:v>0.25463106728435353</c:v>
-                </c:pt>
-                <c:pt idx="1" formatCode="0.00">
-                  <c:v>0.25365530303030304</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="0.00">
-                  <c:v>0.25278396436525613</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="0.00">
-                  <c:v>0.251917012031876</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="0.00">
-                  <c:v>0.25143776166010628</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="0.00">
-                  <c:v>0.25134338815316193</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="0.00">
-                  <c:v>0.24932826142265854</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="0.00">
-                  <c:v>0.24847712753786311</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="0.00">
-                  <c:v>0.24990981128789483</c:v>
-                </c:pt>
-                <c:pt idx="9" formatCode="0.00">
-                  <c:v>0.24832202321355731</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="0.00">
-                  <c:v>0.2482560474528098</c:v>
-                </c:pt>
-                <c:pt idx="11" formatCode="0.00">
-                  <c:v>0.24890196685767385</c:v>
-                </c:pt>
-                <c:pt idx="12" formatCode="0.00">
-                  <c:v>0.24997822435139677</c:v>
+                <c:pt idx="0" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>5.01962301369863</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>4.9976071232876711</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>4.9755912328767122</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>4.9535753424657534</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>4.9425673972602748</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>4.9425673972602748</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>4.8875276712328777</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>4.8655117808219179</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>4.9095435616438357</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>4.8655117808219179</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>4.8655117808219179</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>4.8875276712328777</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>4.9205515068493151</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3047,7 +3560,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>PLANILHAS!$A$7</c:f>
+              <c:f>GRAFICO!$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3085,11 +3598,11 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PLANILHAS!$B$2:$AC$3</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$2:$AC$3</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(PLANILHAS!$E$2:$E$3,PLANILHAS!$G$2:$G$3,PLANILHAS!$I$2:$I$3,PLANILHAS!$K$2:$K$3,PLANILHAS!$M$2:$M$3,PLANILHAS!$O$2:$O$3,PLANILHAS!$Q$2:$Q$3,PLANILHAS!$S$2:$S$3,PLANILHAS!$U$2:$U$3,PLANILHAS!$W$2:$W$3,PLANILHAS!$Y$2:$Y$3,PLANILHAS!$AA$2:$AA$3,PLANILHAS!$AC$2:$AC$3)</c:f>
+              <c:f>(GRAFICO!$E$2:$E$3,GRAFICO!$G$2:$G$3,GRAFICO!$I$2:$I$3,GRAFICO!$K$2:$K$3,GRAFICO!$M$2:$M$3,GRAFICO!$O$2:$O$3,GRAFICO!$Q$2:$Q$3,GRAFICO!$S$2:$S$3,GRAFICO!$U$2:$U$3,GRAFICO!$W$2:$W$3,GRAFICO!$Y$2:$Y$3,GRAFICO!$AA$2:$AA$3,GRAFICO!$AC$2:$AC$3)</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="13"/>
                 <c:lvl>
@@ -3182,52 +3695,52 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>PLANILHAS!$B$7:$AC$7</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$7:$AC$7</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(PLANILHAS!$E$7,PLANILHAS!$G$7,PLANILHAS!$I$7,PLANILHAS!$K$7,PLANILHAS!$M$7,PLANILHAS!$O$7,PLANILHAS!$Q$7,PLANILHAS!$S$7,PLANILHAS!$U$7,PLANILHAS!$W$7,PLANILHAS!$Y$7,PLANILHAS!$AA$7,PLANILHAS!$AC$7)</c:f>
+              <c:f>(GRAFICO!$E$7,GRAFICO!$G$7,GRAFICO!$I$7,GRAFICO!$K$7,GRAFICO!$M$7,GRAFICO!$O$7,GRAFICO!$Q$7,GRAFICO!$S$7,GRAFICO!$U$7,GRAFICO!$W$7,GRAFICO!$Y$7,GRAFICO!$AA$7,GRAFICO!$AC$7)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="13"/>
-                <c:pt idx="0" formatCode="0.00">
-                  <c:v>0.25</c:v>
-                </c:pt>
-                <c:pt idx="1" formatCode="0.00">
-                  <c:v>0.24904081569405279</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="0.00">
-                  <c:v>0.248187040583112</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="0.00">
-                  <c:v>0.24733605422076124</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="0.00">
-                  <c:v>0.24686647496866476</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="0.00">
-                  <c:v>0.24677398551748281</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="0.00">
-                  <c:v>0.24479388792084519</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="0.00">
-                  <c:v>0.24396004736027202</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="0.00">
-                  <c:v>0.2453694373706099</c:v>
-                </c:pt>
-                <c:pt idx="9" formatCode="0.00">
-                  <c:v>0.24380904992202529</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="0.00">
-                  <c:v>0.24374545013346274</c:v>
-                </c:pt>
-                <c:pt idx="11" formatCode="0.00">
-                  <c:v>0.24438294507633357</c:v>
-                </c:pt>
-                <c:pt idx="12" formatCode="0.00">
-                  <c:v>0.24544138398665863</c:v>
+                <c:pt idx="0" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>4.8875276712328777</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>4.8655117808219179</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>4.8434958904109591</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>4.8214800000000002</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>4.8104720547945208</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>4.8104720547945208</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>4.7554323287671245</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>4.7334164383561648</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>4.7774482191780825</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>4.7334164383561648</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>4.7334164383561648</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>4.7554323287671245</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>4.788456164383561</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3244,8 +3757,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="652661872"/>
-        <c:axId val="652637936"/>
+        <c:axId val="1206596736"/>
+        <c:axId val="1206591840"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -3257,7 +3770,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>PLANILHAS!$A$4</c15:sqref>
+                          <c15:sqref>GRAFICO!$A$4</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -3298,10 +3811,10 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>PLANILHAS!$B$2:$AC$3</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$2:$AC$3</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(PLANILHAS!$E$2:$E$3,PLANILHAS!$G$2:$G$3,PLANILHAS!$I$2:$I$3,PLANILHAS!$K$2:$K$3,PLANILHAS!$M$2:$M$3,PLANILHAS!$O$2:$O$3,PLANILHAS!$Q$2:$Q$3,PLANILHAS!$S$2:$S$3,PLANILHAS!$U$2:$U$3,PLANILHAS!$W$2:$W$3,PLANILHAS!$Y$2:$Y$3,PLANILHAS!$AA$2:$AA$3,PLANILHAS!$AC$2:$AC$3)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$E$2:$E$3,GRAFICO!$G$2:$G$3,GRAFICO!$I$2:$I$3,GRAFICO!$K$2:$K$3,GRAFICO!$M$2:$M$3,GRAFICO!$O$2:$O$3,GRAFICO!$Q$2:$Q$3,GRAFICO!$S$2:$S$3,GRAFICO!$U$2:$U$3,GRAFICO!$W$2:$W$3,GRAFICO!$Y$2:$Y$3,GRAFICO!$AA$2:$AA$3,GRAFICO!$AC$2:$AC$3)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -3397,10 +3910,10 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>PLANILHAS!$B$4:$AC$4</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$4:$AC$4</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(PLANILHAS!$E$4,PLANILHAS!$G$4,PLANILHAS!$I$4,PLANILHAS!$K$4,PLANILHAS!$M$4,PLANILHAS!$O$4,PLANILHAS!$Q$4,PLANILHAS!$S$4,PLANILHAS!$U$4,PLANILHAS!$W$4,PLANILHAS!$Y$4,PLANILHAS!$AA$4,PLANILHAS!$AC$4)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$E$4,GRAFICO!$G$4,GRAFICO!$I$4,GRAFICO!$K$4,GRAFICO!$M$4,GRAFICO!$O$4,GRAFICO!$Q$4,GRAFICO!$S$4,GRAFICO!$U$4,GRAFICO!$W$4,GRAFICO!$Y$4,GRAFICO!$AA$4,GRAFICO!$AC$4)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -3458,10 +3971,10 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>PLANILHAS!$A$5</c15:sqref>
+                          <c15:sqref>GRAFICO!$A$5</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -3502,10 +4015,10 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>PLANILHAS!$B$2:$AC$3</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$2:$AC$3</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(PLANILHAS!$E$2:$E$3,PLANILHAS!$G$2:$G$3,PLANILHAS!$I$2:$I$3,PLANILHAS!$K$2:$K$3,PLANILHAS!$M$2:$M$3,PLANILHAS!$O$2:$O$3,PLANILHAS!$Q$2:$Q$3,PLANILHAS!$S$2:$S$3,PLANILHAS!$U$2:$U$3,PLANILHAS!$W$2:$W$3,PLANILHAS!$Y$2:$Y$3,PLANILHAS!$AA$2:$AA$3,PLANILHAS!$AC$2:$AC$3)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$E$2:$E$3,GRAFICO!$G$2:$G$3,GRAFICO!$I$2:$I$3,GRAFICO!$K$2:$K$3,GRAFICO!$M$2:$M$3,GRAFICO!$O$2:$O$3,GRAFICO!$Q$2:$Q$3,GRAFICO!$S$2:$S$3,GRAFICO!$U$2:$U$3,GRAFICO!$W$2:$W$3,GRAFICO!$Y$2:$Y$3,GRAFICO!$AA$2:$AA$3,GRAFICO!$AC$2:$AC$3)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -3601,10 +4114,10 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>PLANILHAS!$B$5:$AC$5</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$5:$AC$5</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(PLANILHAS!$E$5,PLANILHAS!$G$5,PLANILHAS!$I$5,PLANILHAS!$K$5,PLANILHAS!$M$5,PLANILHAS!$O$5,PLANILHAS!$Q$5,PLANILHAS!$S$5,PLANILHAS!$U$5,PLANILHAS!$W$5,PLANILHAS!$Y$5,PLANILHAS!$AA$5,PLANILHAS!$AC$5)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$E$5,GRAFICO!$G$5,GRAFICO!$I$5,GRAFICO!$K$5,GRAFICO!$M$5,GRAFICO!$O$5,GRAFICO!$Q$5,GRAFICO!$S$5,GRAFICO!$U$5,GRAFICO!$W$5,GRAFICO!$Y$5,GRAFICO!$AA$5,GRAFICO!$AC$5)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -3660,7 +4173,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="652661872"/>
+        <c:axId val="1206596736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3703,7 +4216,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="652637936"/>
+        <c:crossAx val="1206591840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3711,7 +4224,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="652637936"/>
+        <c:axId val="1206591840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3762,7 +4275,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="652661872"/>
+        <c:crossAx val="1206596736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6157,6 +6670,7 @@
       <sheetName val="160519"/>
       <sheetName val="170519"/>
       <sheetName val="200519"/>
+      <sheetName val="210519"/>
       <sheetName val="COMPARAÇÃO DIA A DIA"/>
       <sheetName val="TESOURO IPCA"/>
       <sheetName val="TESOURO IPCA JUROS SEMESTRAIS"/>
@@ -6194,6 +6708,7 @@
       <sheetData sheetId="15"/>
       <sheetData sheetId="16"/>
       <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6216,6 +6731,7 @@
       <sheetName val="160519"/>
       <sheetName val="170519"/>
       <sheetName val="200519"/>
+      <sheetName val="210519"/>
       <sheetName val="COMPARAÇÃO DIA A DIA"/>
       <sheetName val="TESOURO IPCA"/>
       <sheetName val="TESOURO IPCA JUROS SEMESTRAIS"/>
@@ -6251,6 +6767,7 @@
       <sheetData sheetId="17"/>
       <sheetData sheetId="18"/>
       <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6546,7 +7063,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6614,16 +7131,16 @@
         <v>4.5599999999999996</v>
       </c>
       <c r="H2" s="6">
-        <f>PLANILHAS!AC4</f>
+        <f>GRAFICO!AC4</f>
         <v>1607.3</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D10" s="47"/>
+      <c r="D10" s="45"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D11" s="12"/>
-      <c r="E11" s="46"/>
+      <c r="E11" s="44"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6633,10 +7150,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AI11"/>
+  <dimension ref="A2:DP11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:AC7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6672,296 +7189,558 @@
     <col min="29" max="29" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="120" width="9.140625" style="48"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:35" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22" t="s">
+    <row r="2" spans="1:120" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="23" t="s">
+      <c r="H2" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="23" t="s">
+      <c r="I2" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="23" t="s">
+      <c r="J2" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="23" t="s">
+      <c r="K2" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="24" t="s">
+      <c r="L2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="24" t="s">
+      <c r="M2" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="24" t="s">
+      <c r="N2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="24" t="s">
+      <c r="O2" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="P2" s="24" t="s">
+      <c r="P2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="Q2" s="24" t="s">
+      <c r="Q2" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="R2" s="24" t="s">
+      <c r="R2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="24" t="s">
+      <c r="S2" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="T2" s="24" t="s">
+      <c r="T2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="U2" s="24" t="s">
+      <c r="U2" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="V2" s="24" t="s">
+      <c r="V2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="W2" s="24" t="s">
+      <c r="W2" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="X2" s="24" t="s">
+      <c r="X2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="Y2" s="24" t="s">
+      <c r="Y2" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="Z2" s="24" t="s">
+      <c r="Z2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="24" t="s">
+      <c r="AA2" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="AB2" s="24" t="s">
+      <c r="AB2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="AC2" s="24" t="s">
+      <c r="AC2" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="AD2" s="24" t="s">
+      <c r="AD2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="AE2" s="24" t="s">
+      <c r="AE2" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="AF2" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="AG2" s="24" t="s">
-        <v>12</v>
-      </c>
+      <c r="AF2" s="47"/>
+      <c r="AG2" s="47"/>
+      <c r="AH2" s="47"/>
+      <c r="AI2" s="47"/>
+      <c r="AJ2" s="47"/>
+      <c r="AK2" s="47"/>
+      <c r="AL2" s="47"/>
+      <c r="AM2" s="47"/>
+      <c r="AN2" s="47"/>
+      <c r="AO2" s="47"/>
+      <c r="AP2" s="47"/>
+      <c r="AQ2" s="47"/>
+      <c r="AR2" s="47"/>
+      <c r="AS2" s="47"/>
+      <c r="AT2" s="47"/>
+      <c r="AU2" s="47"/>
+      <c r="AV2" s="47"/>
+      <c r="AW2" s="47"/>
+      <c r="AX2" s="47"/>
+      <c r="AY2" s="47"/>
+      <c r="AZ2" s="47"/>
+      <c r="BA2" s="47"/>
+      <c r="BB2" s="47"/>
+      <c r="BC2" s="47"/>
+      <c r="BD2" s="47"/>
+      <c r="BE2" s="47"/>
+      <c r="BF2" s="47"/>
+      <c r="BG2" s="47"/>
+      <c r="BH2" s="47"/>
+      <c r="BI2" s="47"/>
+      <c r="BJ2" s="47"/>
+      <c r="BK2" s="47"/>
+      <c r="BL2" s="47"/>
+      <c r="BM2" s="47"/>
+      <c r="BN2" s="47"/>
+      <c r="BO2" s="47"/>
+      <c r="BP2" s="47"/>
+      <c r="BQ2" s="47"/>
+      <c r="BR2" s="47"/>
+      <c r="BS2" s="47"/>
+      <c r="BT2" s="47"/>
+      <c r="BU2" s="47"/>
+      <c r="BV2" s="47"/>
+      <c r="BW2" s="47"/>
+      <c r="BX2" s="47"/>
+      <c r="BY2" s="47"/>
+      <c r="BZ2" s="47"/>
+      <c r="CA2" s="47"/>
+      <c r="CB2" s="47"/>
+      <c r="CC2" s="47"/>
+      <c r="CD2" s="47"/>
+      <c r="CE2" s="47"/>
+      <c r="CF2" s="47"/>
+      <c r="CG2" s="47"/>
+      <c r="CH2" s="47"/>
+      <c r="CI2" s="47"/>
+      <c r="CJ2" s="47"/>
+      <c r="CK2" s="47"/>
+      <c r="CL2" s="47"/>
+      <c r="CM2" s="47"/>
+      <c r="CN2" s="47"/>
+      <c r="CO2" s="47"/>
+      <c r="CP2" s="47"/>
+      <c r="CQ2" s="47"/>
+      <c r="CR2" s="47"/>
+      <c r="CS2" s="47"/>
+      <c r="CT2" s="47"/>
+      <c r="CU2" s="47"/>
+      <c r="CV2" s="47"/>
+      <c r="CW2" s="47"/>
+      <c r="CX2" s="47"/>
+      <c r="CY2" s="47"/>
+      <c r="CZ2" s="47"/>
+      <c r="DA2" s="47"/>
+      <c r="DB2" s="47"/>
+      <c r="DC2" s="47"/>
+      <c r="DD2" s="47"/>
+      <c r="DE2" s="47"/>
+      <c r="DF2" s="47"/>
+      <c r="DG2" s="47"/>
+      <c r="DH2" s="47"/>
+      <c r="DI2" s="47"/>
+      <c r="DJ2" s="47"/>
+      <c r="DK2" s="47"/>
+      <c r="DL2" s="47"/>
+      <c r="DM2" s="47"/>
+      <c r="DN2" s="47"/>
+      <c r="DO2" s="47"/>
+      <c r="DP2" s="47"/>
     </row>
-    <row r="3" spans="1:35" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="35" t="s">
+    <row r="3" spans="1:120" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="25">
+      <c r="C3" s="34"/>
+      <c r="D3" s="23">
         <v>43587</v>
       </c>
-      <c r="E3" s="26">
+      <c r="E3" s="24">
         <v>43587</v>
       </c>
-      <c r="F3" s="27">
+      <c r="F3" s="25">
         <v>43588</v>
       </c>
-      <c r="G3" s="26">
+      <c r="G3" s="24">
         <v>43588</v>
       </c>
-      <c r="H3" s="27">
+      <c r="H3" s="25">
         <v>43591</v>
       </c>
-      <c r="I3" s="25">
+      <c r="I3" s="23">
         <v>43591</v>
       </c>
-      <c r="J3" s="28">
+      <c r="J3" s="26">
         <v>43592</v>
       </c>
-      <c r="K3" s="29">
+      <c r="K3" s="27">
         <v>43592</v>
       </c>
-      <c r="L3" s="30">
+      <c r="L3" s="28">
         <v>43593</v>
       </c>
-      <c r="M3" s="31">
+      <c r="M3" s="29">
         <v>43593</v>
       </c>
-      <c r="N3" s="30">
+      <c r="N3" s="28">
         <v>43594</v>
       </c>
-      <c r="O3" s="31">
+      <c r="O3" s="29">
         <v>43594</v>
       </c>
-      <c r="P3" s="30">
+      <c r="P3" s="28">
         <v>43595</v>
       </c>
-      <c r="Q3" s="31">
+      <c r="Q3" s="29">
         <v>43595</v>
       </c>
-      <c r="R3" s="30">
+      <c r="R3" s="28">
         <v>43598</v>
       </c>
-      <c r="S3" s="31">
+      <c r="S3" s="29">
         <v>43598</v>
       </c>
-      <c r="T3" s="30">
+      <c r="T3" s="28">
         <v>43599</v>
       </c>
-      <c r="U3" s="31">
+      <c r="U3" s="29">
         <v>43599</v>
       </c>
-      <c r="V3" s="30">
+      <c r="V3" s="28">
         <v>43600</v>
       </c>
-      <c r="W3" s="31">
+      <c r="W3" s="29">
         <v>43600</v>
       </c>
-      <c r="X3" s="30">
+      <c r="X3" s="28">
         <v>43601</v>
       </c>
-      <c r="Y3" s="31">
+      <c r="Y3" s="29">
         <v>43601</v>
       </c>
-      <c r="Z3" s="30">
+      <c r="Z3" s="28">
         <v>43602</v>
       </c>
-      <c r="AA3" s="31">
+      <c r="AA3" s="29">
         <v>43602</v>
       </c>
-      <c r="AB3" s="30">
+      <c r="AB3" s="28">
         <v>43605</v>
       </c>
-      <c r="AC3" s="32">
+      <c r="AC3" s="30">
         <v>43605</v>
       </c>
-      <c r="AD3" s="30"/>
-      <c r="AE3" s="31"/>
-      <c r="AF3" s="30"/>
-      <c r="AG3" s="31"/>
+      <c r="AD3" s="28">
+        <v>43606</v>
+      </c>
+      <c r="AE3" s="29">
+        <v>43606</v>
+      </c>
+      <c r="AF3" s="47"/>
+      <c r="AG3" s="47"/>
+      <c r="AH3" s="47"/>
+      <c r="AI3" s="47"/>
+      <c r="AJ3" s="47"/>
+      <c r="AK3" s="47"/>
+      <c r="AL3" s="47"/>
+      <c r="AM3" s="47"/>
+      <c r="AN3" s="47"/>
+      <c r="AO3" s="47"/>
+      <c r="AP3" s="47"/>
+      <c r="AQ3" s="47"/>
+      <c r="AR3" s="47"/>
+      <c r="AS3" s="47"/>
+      <c r="AT3" s="47"/>
+      <c r="AU3" s="47"/>
+      <c r="AV3" s="47"/>
+      <c r="AW3" s="47"/>
+      <c r="AX3" s="47"/>
+      <c r="AY3" s="47"/>
+      <c r="AZ3" s="47"/>
+      <c r="BA3" s="47"/>
+      <c r="BB3" s="47"/>
+      <c r="BC3" s="47"/>
+      <c r="BD3" s="47"/>
+      <c r="BE3" s="47"/>
+      <c r="BF3" s="47"/>
+      <c r="BG3" s="47"/>
+      <c r="BH3" s="47"/>
+      <c r="BI3" s="47"/>
+      <c r="BJ3" s="47"/>
+      <c r="BK3" s="47"/>
+      <c r="BL3" s="47"/>
+      <c r="BM3" s="47"/>
+      <c r="BN3" s="47"/>
+      <c r="BO3" s="47"/>
+      <c r="BP3" s="47"/>
+      <c r="BQ3" s="47"/>
+      <c r="BR3" s="47"/>
+      <c r="BS3" s="47"/>
+      <c r="BT3" s="47"/>
+      <c r="BU3" s="47"/>
+      <c r="BV3" s="47"/>
+      <c r="BW3" s="47"/>
+      <c r="BX3" s="47"/>
+      <c r="BY3" s="47"/>
+      <c r="BZ3" s="47"/>
+      <c r="CA3" s="47"/>
+      <c r="CB3" s="47"/>
+      <c r="CC3" s="47"/>
+      <c r="CD3" s="47"/>
+      <c r="CE3" s="47"/>
+      <c r="CF3" s="47"/>
+      <c r="CG3" s="47"/>
+      <c r="CH3" s="47"/>
+      <c r="CI3" s="47"/>
+      <c r="CJ3" s="47"/>
+      <c r="CK3" s="47"/>
+      <c r="CL3" s="47"/>
+      <c r="CM3" s="47"/>
+      <c r="CN3" s="47"/>
+      <c r="CO3" s="47"/>
+      <c r="CP3" s="47"/>
+      <c r="CQ3" s="47"/>
+      <c r="CR3" s="47"/>
+      <c r="CS3" s="47"/>
+      <c r="CT3" s="47"/>
+      <c r="CU3" s="47"/>
+      <c r="CV3" s="47"/>
+      <c r="CW3" s="47"/>
+      <c r="CX3" s="47"/>
+      <c r="CY3" s="47"/>
+      <c r="CZ3" s="47"/>
+      <c r="DA3" s="47"/>
+      <c r="DB3" s="47"/>
+      <c r="DC3" s="47"/>
+      <c r="DD3" s="47"/>
+      <c r="DE3" s="47"/>
+      <c r="DF3" s="47"/>
+      <c r="DG3" s="47"/>
+      <c r="DH3" s="47"/>
+      <c r="DI3" s="47"/>
+      <c r="DJ3" s="47"/>
+      <c r="DK3" s="47"/>
+      <c r="DL3" s="47"/>
+      <c r="DM3" s="47"/>
+      <c r="DN3" s="47"/>
+      <c r="DO3" s="47"/>
+      <c r="DP3" s="47"/>
     </row>
-    <row r="4" spans="1:35" s="44" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="45" t="s">
+    <row r="4" spans="1:120" s="42" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="38">
+      <c r="C4" s="36">
         <v>49444</v>
       </c>
-      <c r="D4" s="39">
+      <c r="D4" s="37">
         <v>4.5599999999999996</v>
       </c>
-      <c r="E4" s="40">
+      <c r="E4" s="38">
         <v>1577.93</v>
       </c>
-      <c r="F4" s="39">
+      <c r="F4" s="37">
         <v>4.54</v>
       </c>
-      <c r="G4" s="40">
+      <c r="G4" s="38">
         <v>1584</v>
       </c>
-      <c r="H4" s="39">
+      <c r="H4" s="37">
         <v>4.5199999999999996</v>
       </c>
-      <c r="I4" s="40">
+      <c r="I4" s="38">
         <v>1589.46</v>
       </c>
-      <c r="J4" s="41">
+      <c r="J4" s="39">
         <v>4.5</v>
       </c>
-      <c r="K4" s="42">
+      <c r="K4" s="40">
         <v>1594.93</v>
       </c>
-      <c r="L4" s="41">
+      <c r="L4" s="39">
         <v>4.49</v>
       </c>
-      <c r="M4" s="42">
+      <c r="M4" s="40">
         <v>1597.97</v>
       </c>
-      <c r="N4" s="41">
+      <c r="N4" s="39">
         <v>4.49</v>
       </c>
-      <c r="O4" s="42">
+      <c r="O4" s="40">
         <v>1598.57</v>
       </c>
-      <c r="P4" s="41">
+      <c r="P4" s="39">
         <v>4.4400000000000004</v>
       </c>
-      <c r="Q4" s="42">
+      <c r="Q4" s="40">
         <v>1611.49</v>
       </c>
-      <c r="R4" s="41">
+      <c r="R4" s="39">
         <v>4.42</v>
       </c>
-      <c r="S4" s="42">
+      <c r="S4" s="40">
         <v>1617.01</v>
       </c>
-      <c r="T4" s="41">
+      <c r="T4" s="39">
         <v>4.46</v>
       </c>
-      <c r="U4" s="42">
+      <c r="U4" s="40">
         <v>1607.74</v>
       </c>
-      <c r="V4" s="41">
+      <c r="V4" s="39">
         <v>4.42</v>
       </c>
-      <c r="W4" s="42">
+      <c r="W4" s="40">
         <v>1618.02</v>
       </c>
-      <c r="X4" s="41">
+      <c r="X4" s="39">
         <v>4.42</v>
       </c>
-      <c r="Y4" s="42">
+      <c r="Y4" s="40">
         <v>1618.45</v>
       </c>
-      <c r="Z4" s="41">
+      <c r="Z4" s="39">
         <v>4.4400000000000004</v>
       </c>
-      <c r="AA4" s="43">
+      <c r="AA4" s="41">
         <v>1614.25</v>
       </c>
-      <c r="AB4" s="41">
+      <c r="AB4" s="39">
         <v>4.47</v>
       </c>
-      <c r="AC4" s="42">
+      <c r="AC4" s="40">
         <v>1607.3</v>
       </c>
-      <c r="AD4" s="32"/>
-      <c r="AE4" s="31"/>
-      <c r="AF4" s="30"/>
-      <c r="AG4" s="31"/>
+      <c r="AD4" s="39">
+        <v>4.29</v>
+      </c>
+      <c r="AE4" s="40">
+        <v>1652.51</v>
+      </c>
+      <c r="AF4" s="47"/>
+      <c r="AG4" s="47"/>
+      <c r="AH4" s="47"/>
+      <c r="AI4" s="47"/>
+      <c r="AJ4" s="47"/>
+      <c r="AK4" s="47"/>
+      <c r="AL4" s="47"/>
+      <c r="AM4" s="47"/>
+      <c r="AN4" s="47"/>
+      <c r="AO4" s="47"/>
+      <c r="AP4" s="47"/>
+      <c r="AQ4" s="47"/>
+      <c r="AR4" s="47"/>
+      <c r="AS4" s="47"/>
+      <c r="AT4" s="47"/>
+      <c r="AU4" s="47"/>
+      <c r="AV4" s="47"/>
+      <c r="AW4" s="47"/>
+      <c r="AX4" s="47"/>
+      <c r="AY4" s="47"/>
+      <c r="AZ4" s="47"/>
+      <c r="BA4" s="47"/>
+      <c r="BB4" s="47"/>
+      <c r="BC4" s="47"/>
+      <c r="BD4" s="47"/>
+      <c r="BE4" s="47"/>
+      <c r="BF4" s="47"/>
+      <c r="BG4" s="47"/>
+      <c r="BH4" s="47"/>
+      <c r="BI4" s="47"/>
+      <c r="BJ4" s="47"/>
+      <c r="BK4" s="47"/>
+      <c r="BL4" s="47"/>
+      <c r="BM4" s="47"/>
+      <c r="BN4" s="47"/>
+      <c r="BO4" s="47"/>
+      <c r="BP4" s="47"/>
+      <c r="BQ4" s="47"/>
+      <c r="BR4" s="47"/>
+      <c r="BS4" s="47"/>
+      <c r="BT4" s="47"/>
+      <c r="BU4" s="47"/>
+      <c r="BV4" s="47"/>
+      <c r="BW4" s="47"/>
+      <c r="BX4" s="47"/>
+      <c r="BY4" s="47"/>
+      <c r="BZ4" s="47"/>
+      <c r="CA4" s="47"/>
+      <c r="CB4" s="47"/>
+      <c r="CC4" s="47"/>
+      <c r="CD4" s="47"/>
+      <c r="CE4" s="47"/>
+      <c r="CF4" s="47"/>
+      <c r="CG4" s="47"/>
+      <c r="CH4" s="47"/>
+      <c r="CI4" s="47"/>
+      <c r="CJ4" s="47"/>
+      <c r="CK4" s="47"/>
+      <c r="CL4" s="47"/>
+      <c r="CM4" s="47"/>
+      <c r="CN4" s="47"/>
+      <c r="CO4" s="47"/>
+      <c r="CP4" s="47"/>
+      <c r="CQ4" s="47"/>
+      <c r="CR4" s="47"/>
+      <c r="CS4" s="47"/>
+      <c r="CT4" s="47"/>
+      <c r="CU4" s="47"/>
+      <c r="CV4" s="47"/>
+      <c r="CW4" s="47"/>
+      <c r="CX4" s="47"/>
+      <c r="CY4" s="47"/>
+      <c r="CZ4" s="47"/>
+      <c r="DA4" s="47"/>
+      <c r="DB4" s="47"/>
+      <c r="DC4" s="47"/>
+      <c r="DD4" s="47"/>
+      <c r="DE4" s="47"/>
+      <c r="DF4" s="47"/>
+      <c r="DG4" s="47"/>
+      <c r="DH4" s="47"/>
+      <c r="DI4" s="47"/>
+      <c r="DJ4" s="47"/>
+      <c r="DK4" s="47"/>
+      <c r="DL4" s="47"/>
+      <c r="DM4" s="47"/>
+      <c r="DN4" s="47"/>
+      <c r="DO4" s="47"/>
+      <c r="DP4" s="47"/>
     </row>
-    <row r="5" spans="1:35" s="49" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="34" t="s">
+    <row r="5" spans="1:120" s="47" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="31" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="13">
@@ -7045,249 +7824,265 @@
       <c r="AC5" s="18">
         <v>1637.01</v>
       </c>
-      <c r="AD5" s="14"/>
-      <c r="AE5" s="19"/>
-      <c r="AF5" s="20"/>
-      <c r="AG5" s="14"/>
-      <c r="AH5" s="19"/>
-      <c r="AI5" s="20"/>
+      <c r="AD5" s="51">
+        <v>4.41</v>
+      </c>
+      <c r="AE5" s="52">
+        <v>1622.51</v>
+      </c>
     </row>
-    <row r="6" spans="1:35" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="48" t="s">
+    <row r="6" spans="1:120" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="51">
+      <c r="B6" s="49">
         <f>'020519'!C2</f>
         <v>401.79</v>
       </c>
-      <c r="C6" s="52">
+      <c r="C6" s="50">
         <v>43587</v>
       </c>
-      <c r="D6" s="51">
+      <c r="D6" s="56">
+        <f>$B$6/E4</f>
+        <v>0.25463106728435353</v>
+      </c>
+      <c r="E6" s="54">
         <f>(D4/365)*$B$6</f>
         <v>5.01962301369863</v>
       </c>
-      <c r="E6" s="53">
-        <f>$B$6/E4</f>
-        <v>0.25463106728435353</v>
-      </c>
-      <c r="F6" s="51">
-        <f>(F4/365)*$B$6</f>
+      <c r="F6" s="56">
+        <f t="shared" ref="F6:AE6" si="0">$B$6/G4</f>
+        <v>0.25365530303030304</v>
+      </c>
+      <c r="G6" s="54">
+        <f t="shared" ref="G6:AE6" si="1">(F4/365)*$B$6</f>
         <v>4.9976071232876711</v>
       </c>
-      <c r="G6" s="53">
-        <f>$B$6/G4</f>
-        <v>0.25365530303030304</v>
-      </c>
-      <c r="H6" s="51">
-        <f t="shared" ref="H6:AC6" si="0">(H4/365)*$B$6</f>
+      <c r="H6" s="56">
+        <f t="shared" ref="H6:AE6" si="2">$B$6/I4</f>
+        <v>0.25278396436525613</v>
+      </c>
+      <c r="I6" s="54">
+        <f t="shared" ref="I6:AE6" si="3">(H4/365)*$B$6</f>
         <v>4.9755912328767122</v>
       </c>
-      <c r="I6" s="53">
-        <f t="shared" ref="I6:AC6" si="1">$B$6/I4</f>
-        <v>0.25278396436525613</v>
-      </c>
-      <c r="J6" s="51">
-        <f t="shared" ref="J6:AC6" si="2">(J4/365)*$B$6</f>
+      <c r="J6" s="56">
+        <f t="shared" ref="J6:AE6" si="4">$B$6/K4</f>
+        <v>0.251917012031876</v>
+      </c>
+      <c r="K6" s="54">
+        <f t="shared" ref="K6:AE6" si="5">(J4/365)*$B$6</f>
         <v>4.9535753424657534</v>
       </c>
-      <c r="K6" s="53">
-        <f t="shared" ref="K6:AC6" si="3">$B$6/K4</f>
-        <v>0.251917012031876</v>
-      </c>
-      <c r="L6" s="51">
-        <f t="shared" ref="L6:AC6" si="4">(L4/365)*$B$6</f>
+      <c r="L6" s="56">
+        <f t="shared" ref="L6:AE6" si="6">$B$6/M4</f>
+        <v>0.25143776166010628</v>
+      </c>
+      <c r="M6" s="54">
+        <f t="shared" ref="M6:AE6" si="7">(L4/365)*$B$6</f>
         <v>4.9425673972602748</v>
       </c>
-      <c r="M6" s="53">
-        <f t="shared" ref="M6:AC6" si="5">$B$6/M4</f>
-        <v>0.25143776166010628</v>
-      </c>
-      <c r="N6" s="51">
-        <f t="shared" ref="N6:AC6" si="6">(N4/365)*$B$6</f>
+      <c r="N6" s="56">
+        <f t="shared" ref="N6:AE6" si="8">$B$6/O4</f>
+        <v>0.25134338815316193</v>
+      </c>
+      <c r="O6" s="54">
+        <f t="shared" ref="O6:AE6" si="9">(N4/365)*$B$6</f>
         <v>4.9425673972602748</v>
       </c>
-      <c r="O6" s="53">
-        <f t="shared" ref="O6:AC6" si="7">$B$6/O4</f>
-        <v>0.25134338815316193</v>
-      </c>
-      <c r="P6" s="51">
-        <f t="shared" ref="P6:AC6" si="8">(P4/365)*$B$6</f>
+      <c r="P6" s="56">
+        <f t="shared" ref="P6:AE6" si="10">$B$6/Q4</f>
+        <v>0.24932826142265854</v>
+      </c>
+      <c r="Q6" s="54">
+        <f t="shared" ref="Q6:AE6" si="11">(P4/365)*$B$6</f>
         <v>4.8875276712328777</v>
       </c>
-      <c r="Q6" s="53">
-        <f t="shared" ref="Q6:AC6" si="9">$B$6/Q4</f>
-        <v>0.24932826142265854</v>
-      </c>
-      <c r="R6" s="51">
-        <f t="shared" ref="R6:AC6" si="10">(R4/365)*$B$6</f>
+      <c r="R6" s="56">
+        <f t="shared" ref="R6:AE6" si="12">$B$6/S4</f>
+        <v>0.24847712753786311</v>
+      </c>
+      <c r="S6" s="54">
+        <f t="shared" ref="S6:AE6" si="13">(R4/365)*$B$6</f>
         <v>4.8655117808219179</v>
       </c>
-      <c r="S6" s="53">
-        <f t="shared" ref="S6:AC6" si="11">$B$6/S4</f>
-        <v>0.24847712753786311</v>
-      </c>
-      <c r="T6" s="51">
-        <f t="shared" ref="T6:AC6" si="12">(T4/365)*$B$6</f>
+      <c r="T6" s="56">
+        <f t="shared" ref="T6:AE6" si="14">$B$6/U4</f>
+        <v>0.24990981128789483</v>
+      </c>
+      <c r="U6" s="54">
+        <f t="shared" ref="U6:AE6" si="15">(T4/365)*$B$6</f>
         <v>4.9095435616438357</v>
       </c>
-      <c r="U6" s="53">
-        <f t="shared" ref="U6:AC6" si="13">$B$6/U4</f>
-        <v>0.24990981128789483</v>
-      </c>
-      <c r="V6" s="51">
-        <f t="shared" ref="V6:AC6" si="14">(V4/365)*$B$6</f>
+      <c r="V6" s="56">
+        <f t="shared" ref="V6:AE6" si="16">$B$6/W4</f>
+        <v>0.24832202321355731</v>
+      </c>
+      <c r="W6" s="54">
+        <f t="shared" ref="W6:AE6" si="17">(V4/365)*$B$6</f>
         <v>4.8655117808219179</v>
       </c>
-      <c r="W6" s="53">
-        <f t="shared" ref="W6:AC6" si="15">$B$6/W4</f>
-        <v>0.24832202321355731</v>
-      </c>
-      <c r="X6" s="51">
-        <f t="shared" ref="X6:AC6" si="16">(X4/365)*$B$6</f>
+      <c r="X6" s="56">
+        <f t="shared" ref="X6:AE6" si="18">$B$6/Y4</f>
+        <v>0.2482560474528098</v>
+      </c>
+      <c r="Y6" s="54">
+        <f t="shared" ref="Y6:AE6" si="19">(X4/365)*$B$6</f>
         <v>4.8655117808219179</v>
       </c>
-      <c r="Y6" s="53">
-        <f t="shared" ref="Y6:AC6" si="17">$B$6/Y4</f>
-        <v>0.2482560474528098</v>
-      </c>
-      <c r="Z6" s="51">
-        <f t="shared" ref="Z6:AC6" si="18">(Z4/365)*$B$6</f>
+      <c r="Z6" s="56">
+        <f t="shared" ref="Z6:AE6" si="20">$B$6/AA4</f>
+        <v>0.24890196685767385</v>
+      </c>
+      <c r="AA6" s="54">
+        <f t="shared" ref="AA6:AE6" si="21">(Z4/365)*$B$6</f>
         <v>4.8875276712328777</v>
       </c>
-      <c r="AA6" s="53">
-        <f t="shared" ref="AA6:AC6" si="19">$B$6/AA4</f>
-        <v>0.24890196685767385</v>
-      </c>
-      <c r="AB6" s="51">
-        <f t="shared" ref="AB6:AC6" si="20">(AB4/365)*$B$6</f>
+      <c r="AB6" s="56">
+        <f t="shared" ref="AB6:AE6" si="22">$B$6/AC4</f>
+        <v>0.24997822435139677</v>
+      </c>
+      <c r="AC6" s="54">
+        <f t="shared" ref="AC6:AE6" si="23">(AB4/365)*$B$6</f>
         <v>4.9205515068493151</v>
       </c>
-      <c r="AC6" s="53">
-        <f t="shared" ref="AC6:AC7" si="21">$B$6/AC4</f>
-        <v>0.24997822435139677</v>
+      <c r="AD6" s="56">
+        <f t="shared" ref="AD6:AE6" si="24">$B$6/AE4</f>
+        <v>0.24313922457352755</v>
+      </c>
+      <c r="AE6" s="54">
+        <f t="shared" ref="AE6:AE7" si="25">(AD4/365)*$B$6</f>
+        <v>4.7224084931506853</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A7" s="48" t="s">
+    <row r="7" spans="1:120" x14ac:dyDescent="0.25">
+      <c r="A7" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="51">
+      <c r="B7" s="49">
         <f>'020519'!C2</f>
         <v>401.79</v>
       </c>
-      <c r="C7" s="52">
+      <c r="C7" s="50">
         <v>43587</v>
       </c>
-      <c r="D7" s="51">
+      <c r="D7" s="55">
+        <f>$B$7/E5</f>
+        <v>0.25</v>
+      </c>
+      <c r="E7" s="54">
         <f>(D5/365)*$B$6</f>
         <v>4.8875276712328777</v>
       </c>
-      <c r="E7" s="53">
-        <f>$B$6/E5</f>
-        <v>0.25</v>
-      </c>
-      <c r="F7" s="51">
-        <f t="shared" ref="F7:AC7" si="22">(F5/365)*$B$6</f>
+      <c r="F7" s="56">
+        <f t="shared" ref="F7:AE7" si="26">$B$7/G5</f>
+        <v>0.24904081569405279</v>
+      </c>
+      <c r="G7" s="54">
+        <f t="shared" ref="G7:AE7" si="27">(F5/365)*$B$6</f>
         <v>4.8655117808219179</v>
       </c>
-      <c r="G7" s="53">
-        <f t="shared" ref="G7:AC7" si="23">$B$6/G5</f>
-        <v>0.24904081569405279</v>
-      </c>
-      <c r="H7" s="51">
-        <f t="shared" ref="H7:AC7" si="24">(H5/365)*$B$6</f>
+      <c r="H7" s="56">
+        <f t="shared" ref="H7:AE7" si="28">$B$7/I5</f>
+        <v>0.248187040583112</v>
+      </c>
+      <c r="I7" s="54">
+        <f t="shared" ref="I7:AE7" si="29">(H5/365)*$B$6</f>
         <v>4.8434958904109591</v>
       </c>
-      <c r="I7" s="53">
-        <f t="shared" ref="I7:AC7" si="25">$B$6/I5</f>
-        <v>0.248187040583112</v>
-      </c>
-      <c r="J7" s="51">
-        <f t="shared" ref="J7:AC7" si="26">(J5/365)*$B$6</f>
+      <c r="J7" s="56">
+        <f t="shared" ref="J7:AE7" si="30">$B$7/K5</f>
+        <v>0.24733605422076124</v>
+      </c>
+      <c r="K7" s="54">
+        <f t="shared" ref="K7:AE7" si="31">(J5/365)*$B$6</f>
         <v>4.8214800000000002</v>
       </c>
-      <c r="K7" s="53">
-        <f t="shared" ref="K7:AC7" si="27">$B$6/K5</f>
-        <v>0.24733605422076124</v>
-      </c>
-      <c r="L7" s="51">
-        <f t="shared" ref="L7:AC7" si="28">(L5/365)*$B$6</f>
+      <c r="L7" s="56">
+        <f t="shared" ref="L7:AE7" si="32">$B$7/M5</f>
+        <v>0.24686647496866476</v>
+      </c>
+      <c r="M7" s="54">
+        <f t="shared" ref="M7:AE7" si="33">(L5/365)*$B$6</f>
         <v>4.8104720547945208</v>
       </c>
-      <c r="M7" s="53">
-        <f t="shared" ref="M7:AC7" si="29">$B$6/M5</f>
-        <v>0.24686647496866476</v>
-      </c>
-      <c r="N7" s="51">
-        <f t="shared" ref="N7:AC7" si="30">(N5/365)*$B$6</f>
+      <c r="N7" s="56">
+        <f t="shared" ref="N7:AE7" si="34">$B$7/O5</f>
+        <v>0.24677398551748281</v>
+      </c>
+      <c r="O7" s="54">
+        <f t="shared" ref="O7:AE7" si="35">(N5/365)*$B$6</f>
         <v>4.8104720547945208</v>
       </c>
-      <c r="O7" s="53">
-        <f t="shared" ref="O7:AC7" si="31">$B$6/O5</f>
-        <v>0.24677398551748281</v>
-      </c>
-      <c r="P7" s="51">
-        <f t="shared" ref="P7:AC7" si="32">(P5/365)*$B$6</f>
+      <c r="P7" s="56">
+        <f t="shared" ref="P7:AE7" si="36">$B$7/Q5</f>
+        <v>0.24479388792084519</v>
+      </c>
+      <c r="Q7" s="54">
+        <f t="shared" ref="Q7:AE7" si="37">(P5/365)*$B$6</f>
         <v>4.7554323287671245</v>
       </c>
-      <c r="Q7" s="53">
-        <f t="shared" ref="Q7:AC7" si="33">$B$6/Q5</f>
-        <v>0.24479388792084519</v>
-      </c>
-      <c r="R7" s="51">
-        <f t="shared" ref="R7:AC7" si="34">(R5/365)*$B$6</f>
+      <c r="R7" s="56">
+        <f t="shared" ref="R7:AE7" si="38">$B$7/S5</f>
+        <v>0.24396004736027202</v>
+      </c>
+      <c r="S7" s="54">
+        <f t="shared" ref="S7:AE7" si="39">(R5/365)*$B$6</f>
         <v>4.7334164383561648</v>
       </c>
-      <c r="S7" s="53">
-        <f t="shared" ref="S7:AC7" si="35">$B$6/S5</f>
-        <v>0.24396004736027202</v>
-      </c>
-      <c r="T7" s="51">
-        <f t="shared" ref="T7:AC7" si="36">(T5/365)*$B$6</f>
+      <c r="T7" s="56">
+        <f t="shared" ref="T7:AE7" si="40">$B$7/U5</f>
+        <v>0.2453694373706099</v>
+      </c>
+      <c r="U7" s="54">
+        <f t="shared" ref="U7:AE7" si="41">(T5/365)*$B$6</f>
         <v>4.7774482191780825</v>
       </c>
-      <c r="U7" s="53">
-        <f t="shared" ref="U7:AC7" si="37">$B$6/U5</f>
-        <v>0.2453694373706099</v>
-      </c>
-      <c r="V7" s="51">
-        <f t="shared" ref="V7:AC7" si="38">(V5/365)*$B$6</f>
+      <c r="V7" s="56">
+        <f t="shared" ref="V7:AE7" si="42">$B$7/W5</f>
+        <v>0.24380904992202529</v>
+      </c>
+      <c r="W7" s="54">
+        <f t="shared" ref="W7:AE7" si="43">(V5/365)*$B$6</f>
         <v>4.7334164383561648</v>
       </c>
-      <c r="W7" s="53">
-        <f t="shared" ref="W7:AC7" si="39">$B$6/W5</f>
-        <v>0.24380904992202529</v>
-      </c>
-      <c r="X7" s="51">
-        <f t="shared" ref="X7:AC7" si="40">(X5/365)*$B$6</f>
+      <c r="X7" s="56">
+        <f t="shared" ref="X7:AE7" si="44">$B$7/Y5</f>
+        <v>0.24374545013346274</v>
+      </c>
+      <c r="Y7" s="54">
+        <f t="shared" ref="Y7:AE7" si="45">(X5/365)*$B$6</f>
         <v>4.7334164383561648</v>
       </c>
-      <c r="Y7" s="53">
-        <f t="shared" ref="Y7:AC7" si="41">$B$6/Y5</f>
-        <v>0.24374545013346274</v>
-      </c>
-      <c r="Z7" s="51">
-        <f t="shared" ref="Z7:AC7" si="42">(Z5/365)*$B$6</f>
+      <c r="Z7" s="56">
+        <f t="shared" ref="Z7:AE7" si="46">$B$7/AA5</f>
+        <v>0.24438294507633357</v>
+      </c>
+      <c r="AA7" s="54">
+        <f t="shared" ref="AA7:AE7" si="47">(Z5/365)*$B$6</f>
         <v>4.7554323287671245</v>
       </c>
-      <c r="AA7" s="53">
-        <f t="shared" ref="AA7:AC7" si="43">$B$6/AA5</f>
-        <v>0.24438294507633357</v>
-      </c>
-      <c r="AB7" s="51">
-        <f t="shared" ref="AB7:AC7" si="44">(AB5/365)*$B$6</f>
+      <c r="AB7" s="56">
+        <f t="shared" ref="AB7:AE7" si="48">$B$7/AC5</f>
+        <v>0.24544138398665863</v>
+      </c>
+      <c r="AC7" s="54">
+        <f t="shared" ref="AC7:AE7" si="49">(AB5/365)*$B$6</f>
         <v>4.788456164383561</v>
       </c>
-      <c r="AC7" s="53">
-        <f t="shared" si="21"/>
-        <v>0.24544138398665863</v>
+      <c r="AD7" s="56">
+        <f t="shared" ref="AD7:AE7" si="50">$B$7/AE5</f>
+        <v>0.24763483738158781</v>
+      </c>
+      <c r="AE7" s="54">
+        <f t="shared" si="25"/>
+        <v>4.8545038356164385</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:120" x14ac:dyDescent="0.25">
       <c r="AC10" s="6"/>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:120" x14ac:dyDescent="0.25">
       <c r="AC11" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit atualizacao tesouro 24/05
</commit_message>
<xml_diff>
--- a/TITULO COMPRADO - LIVIO.xlsx
+++ b/TITULO COMPRADO - LIVIO.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="18">
   <si>
     <t>DATA COMPRA</t>
   </si>
@@ -542,15 +542,15 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:idx val="0"/>
+          <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>GRAFICO!$A$6</c:f>
+              <c:f>GRAFICO!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>TITULO VENDA</c:v>
+                  <c:v>VENDA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -558,7 +558,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -569,11 +569,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent3"/>
+                  <a:schemeClr val="accent1"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -584,13 +584,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$2:$AG$3</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$2:$AK$3</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$D$2:$D$3,GRAFICO!$F$2:$F$3,GRAFICO!$H$2:$H$3,GRAFICO!$J$2:$J$3,GRAFICO!$L$2:$L$3,GRAFICO!$N$2:$N$3,GRAFICO!$P$2:$P$3,GRAFICO!$R$2:$R$3,GRAFICO!$T$2:$T$3,GRAFICO!$V$2:$V$3,GRAFICO!$X$2:$X$3,GRAFICO!$Z$2:$Z$3,GRAFICO!$AB$2:$AB$3,GRAFICO!$AD$2:$AD$3,GRAFICO!$AF$2:$AF$3)</c:f>
+              <c:f>(GRAFICO!$D$2:$D$3,GRAFICO!$F$2:$F$3,GRAFICO!$H$2:$H$3,GRAFICO!$J$2:$J$3,GRAFICO!$L$2:$L$3,GRAFICO!$N$2:$N$3,GRAFICO!$P$2:$P$3,GRAFICO!$R$2:$R$3,GRAFICO!$T$2:$T$3,GRAFICO!$V$2:$V$3,GRAFICO!$X$2:$X$3,GRAFICO!$Z$2:$Z$3,GRAFICO!$AB$2:$AB$3,GRAFICO!$AD$2:$AD$3,GRAFICO!$AF$2:$AF$3,GRAFICO!$AH$2:$AH$3,GRAFICO!$AJ$2:$AJ$3)</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="15"/>
+                <c:ptCount val="17"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>02/05</c:v>
@@ -636,6 +636,12 @@
                   </c:pt>
                   <c:pt idx="14">
                     <c:v>22/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>23/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>24/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -682,6 +688,12 @@
                     <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="14">
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
                     <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                 </c:lvl>
@@ -693,58 +705,64 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$6:$AG$6</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$4:$AK$4</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$D$6,GRAFICO!$F$6,GRAFICO!$H$6,GRAFICO!$J$6,GRAFICO!$L$6,GRAFICO!$N$6,GRAFICO!$P$6,GRAFICO!$R$6,GRAFICO!$T$6,GRAFICO!$V$6,GRAFICO!$X$6,GRAFICO!$Z$6,GRAFICO!$AB$6,GRAFICO!$AD$6,GRAFICO!$AF$6)</c:f>
+              <c:f>(GRAFICO!$D$4,GRAFICO!$F$4,GRAFICO!$H$4,GRAFICO!$J$4,GRAFICO!$L$4,GRAFICO!$N$4,GRAFICO!$P$4,GRAFICO!$R$4,GRAFICO!$T$4,GRAFICO!$V$4,GRAFICO!$X$4,GRAFICO!$Z$4,GRAFICO!$AB$4,GRAFICO!$AD$4,GRAFICO!$AF$4,GRAFICO!$AH$4,GRAFICO!$AJ$4)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="15"/>
-                <c:pt idx="0" formatCode="0.00">
-                  <c:v>0.25512798155620736</c:v>
-                </c:pt>
-                <c:pt idx="1" formatCode="0.00">
-                  <c:v>0.2541503130915318</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="0.00">
-                  <c:v>0.25327727400311195</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="0.00">
-                  <c:v>0.25240862980631523</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="0.00">
-                  <c:v>0.25192844417416244</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="0.00">
-                  <c:v>0.25183388649667288</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="0.00">
-                  <c:v>0.24981482723255269</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="0.00">
-                  <c:v>0.2489620323541514</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="0.00">
-                  <c:v>0.2503975119963342</c:v>
-                </c:pt>
-                <c:pt idx="9" formatCode="0.00">
-                  <c:v>0.24880662534269438</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="0.00">
-                  <c:v>0.24874052082979786</c:v>
-                </c:pt>
-                <c:pt idx="11" formatCode="0.00">
-                  <c:v>0.2493877007508046</c:v>
-                </c:pt>
-                <c:pt idx="12" formatCode="0.00">
-                  <c:v>0.25046605856839815</c:v>
-                </c:pt>
-                <c:pt idx="13" formatCode="0.00">
-                  <c:v>0.24361371243561997</c:v>
-                </c:pt>
-                <c:pt idx="14" formatCode="0.00">
-                  <c:v>0.24616698113392466</c:v>
+                <c:ptCount val="17"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>4.5599999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>4.54</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>4.5199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>4.49</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>4.49</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>4.4400000000000004</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>4.42</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>4.46</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>4.42</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>4.42</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>4.4400000000000004</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>4.47</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>4.29</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
+                  <c:v>4.3600000000000003</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="General">
+                  <c:v>4.41</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="General">
+                  <c:v>4.34</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -752,15 +770,15 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
+          <c:idx val="1"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>GRAFICO!$A$7</c:f>
+              <c:f>GRAFICO!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>TITULO COMPRA</c:v>
+                  <c:v>COMPRA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -768,7 +786,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -779,11 +797,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent4"/>
+                  <a:schemeClr val="accent2"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -794,13 +812,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$2:$AG$3</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$2:$AK$3</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$D$2:$D$3,GRAFICO!$F$2:$F$3,GRAFICO!$H$2:$H$3,GRAFICO!$J$2:$J$3,GRAFICO!$L$2:$L$3,GRAFICO!$N$2:$N$3,GRAFICO!$P$2:$P$3,GRAFICO!$R$2:$R$3,GRAFICO!$T$2:$T$3,GRAFICO!$V$2:$V$3,GRAFICO!$X$2:$X$3,GRAFICO!$Z$2:$Z$3,GRAFICO!$AB$2:$AB$3,GRAFICO!$AD$2:$AD$3,GRAFICO!$AF$2:$AF$3)</c:f>
+              <c:f>(GRAFICO!$D$2:$D$3,GRAFICO!$F$2:$F$3,GRAFICO!$H$2:$H$3,GRAFICO!$J$2:$J$3,GRAFICO!$L$2:$L$3,GRAFICO!$N$2:$N$3,GRAFICO!$P$2:$P$3,GRAFICO!$R$2:$R$3,GRAFICO!$T$2:$T$3,GRAFICO!$V$2:$V$3,GRAFICO!$X$2:$X$3,GRAFICO!$Z$2:$Z$3,GRAFICO!$AB$2:$AB$3,GRAFICO!$AD$2:$AD$3,GRAFICO!$AF$2:$AF$3,GRAFICO!$AH$2:$AH$3,GRAFICO!$AJ$2:$AJ$3)</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="15"/>
+                <c:ptCount val="17"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>02/05</c:v>
@@ -846,6 +864,12 @@
                   </c:pt>
                   <c:pt idx="14">
                     <c:v>22/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>23/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>24/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -892,6 +916,12 @@
                     <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="14">
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
                     <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                 </c:lvl>
@@ -903,58 +933,64 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$7:$AG$7</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$5:$AK$5</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$D$7,GRAFICO!$F$7,GRAFICO!$H$7,GRAFICO!$J$7,GRAFICO!$L$7,GRAFICO!$N$7,GRAFICO!$P$7,GRAFICO!$R$7,GRAFICO!$T$7,GRAFICO!$V$7,GRAFICO!$X$7,GRAFICO!$Z$7,GRAFICO!$AB$7,GRAFICO!$AD$7,GRAFICO!$AF$7)</c:f>
+              <c:f>(GRAFICO!$D$5,GRAFICO!$F$5,GRAFICO!$H$5,GRAFICO!$J$5,GRAFICO!$L$5,GRAFICO!$N$5,GRAFICO!$P$5,GRAFICO!$R$5,GRAFICO!$T$5,GRAFICO!$V$5,GRAFICO!$X$5,GRAFICO!$Z$5,GRAFICO!$AB$5,GRAFICO!$AD$5,GRAFICO!$AF$5,GRAFICO!$AH$5,GRAFICO!$AJ$5)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0.25</c:v>
-                </c:pt>
-                <c:pt idx="1" formatCode="0.00">
-                  <c:v>0.24952682055163874</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="0.00">
-                  <c:v>0.24867137929272118</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="0.00">
-                  <c:v>0.24781873222465564</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="0.00">
-                  <c:v>0.2473482365854324</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="0.00">
-                  <c:v>0.24725556664045298</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="0.00">
-                  <c:v>0.24527160486979319</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="0.00">
-                  <c:v>0.24443613706365483</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="0.00">
-                  <c:v>0.24584827750825125</c:v>
-                </c:pt>
-                <c:pt idx="9" formatCode="0.00">
-                  <c:v>0.24428484495287314</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="0.00">
-                  <c:v>0.2442211210488876</c:v>
-                </c:pt>
-                <c:pt idx="11" formatCode="0.00">
-                  <c:v>0.24485986006750585</c:v>
-                </c:pt>
-                <c:pt idx="12" formatCode="0.00">
-                  <c:v>0.24592036452861396</c:v>
-                </c:pt>
-                <c:pt idx="13" formatCode="0.00">
-                  <c:v>0.248118098462867</c:v>
-                </c:pt>
-                <c:pt idx="14" formatCode="0.00">
-                  <c:v>0.24169624280267191</c:v>
+                  <c:v>4.4400000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>4.42</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>4.38</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>4.37</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>4.37</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>4.32</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>4.3</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>4.34</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>4.3</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>4.3</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>4.32</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>4.3499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>4.41</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
+                  <c:v>4.24</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="General">
+                  <c:v>4.29</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="General">
+                  <c:v>4.22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -971,27 +1007,27 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-364703168"/>
-        <c:axId val="-364698816"/>
+        <c:axId val="-545832192"/>
+        <c:axId val="-545829472"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
               <c15:ser>
-                <c:idx val="0"/>
-                <c:order val="0"/>
+                <c:idx val="2"/>
+                <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>GRAFICO!$A$4</c15:sqref>
+                          <c15:sqref>GRAFICO!$A$6</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
                       <c:ptCount val="1"/>
                       <c:pt idx="0">
-                        <c:v>VENDA</c:v>
+                        <c:v>TITULO VENDA</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -999,7 +1035,7 @@
                 <c:spPr>
                   <a:ln w="28575" cap="rnd">
                     <a:solidFill>
-                      <a:schemeClr val="accent1"/>
+                      <a:schemeClr val="accent3"/>
                     </a:solidFill>
                     <a:round/>
                   </a:ln>
@@ -1010,11 +1046,11 @@
                   <c:size val="5"/>
                   <c:spPr>
                     <a:solidFill>
-                      <a:schemeClr val="accent1"/>
+                      <a:schemeClr val="accent3"/>
                     </a:solidFill>
                     <a:ln w="9525">
                       <a:solidFill>
-                        <a:schemeClr val="accent1"/>
+                        <a:schemeClr val="accent3"/>
                       </a:solidFill>
                     </a:ln>
                     <a:effectLst/>
@@ -1025,15 +1061,15 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$2:$AG$3</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$2:$AK$3</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$D$2:$D$3,GRAFICO!$F$2:$F$3,GRAFICO!$H$2:$H$3,GRAFICO!$J$2:$J$3,GRAFICO!$L$2:$L$3,GRAFICO!$N$2:$N$3,GRAFICO!$P$2:$P$3,GRAFICO!$R$2:$R$3,GRAFICO!$T$2:$T$3,GRAFICO!$V$2:$V$3,GRAFICO!$X$2:$X$3,GRAFICO!$Z$2:$Z$3,GRAFICO!$AB$2:$AB$3,GRAFICO!$AD$2:$AD$3,GRAFICO!$AF$2:$AF$3)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$D$2:$D$3,GRAFICO!$F$2:$F$3,GRAFICO!$H$2:$H$3,GRAFICO!$J$2:$J$3,GRAFICO!$L$2:$L$3,GRAFICO!$N$2:$N$3,GRAFICO!$P$2:$P$3,GRAFICO!$R$2:$R$3,GRAFICO!$T$2:$T$3,GRAFICO!$V$2:$V$3,GRAFICO!$X$2:$X$3,GRAFICO!$Z$2:$Z$3,GRAFICO!$AB$2:$AB$3,GRAFICO!$AD$2:$AD$3,GRAFICO!$AF$2:$AF$3,GRAFICO!$AH$2:$AH$3,GRAFICO!$AJ$2:$AJ$3)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:multiLvlStrCache>
-                      <c:ptCount val="15"/>
+                      <c:ptCount val="17"/>
                       <c:lvl>
                         <c:pt idx="0">
                           <c:v>02/05</c:v>
@@ -1079,6 +1115,12 @@
                         </c:pt>
                         <c:pt idx="14">
                           <c:v>22/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="15">
+                          <c:v>23/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="16">
+                          <c:v>24/mai</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
@@ -1125,6 +1167,12 @@
                           <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="14">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="15">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="16">
                           <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                       </c:lvl>
@@ -1136,60 +1184,66 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$4:$AG$4</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$6:$AK$6</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$D$4,GRAFICO!$F$4,GRAFICO!$H$4,GRAFICO!$J$4,GRAFICO!$L$4,GRAFICO!$N$4,GRAFICO!$P$4,GRAFICO!$R$4,GRAFICO!$T$4,GRAFICO!$V$4,GRAFICO!$X$4,GRAFICO!$Z$4,GRAFICO!$AB$4,GRAFICO!$AD$4,GRAFICO!$AF$4)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$D$6,GRAFICO!$F$6,GRAFICO!$H$6,GRAFICO!$J$6,GRAFICO!$L$6,GRAFICO!$N$6,GRAFICO!$P$6,GRAFICO!$R$6,GRAFICO!$T$6,GRAFICO!$V$6,GRAFICO!$X$6,GRAFICO!$Z$6,GRAFICO!$AB$6,GRAFICO!$AD$6,GRAFICO!$AF$6,GRAFICO!$AH$6,GRAFICO!$AJ$6)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>m/d/yyyy</c:formatCode>
-                      <c:ptCount val="15"/>
-                      <c:pt idx="0" formatCode="General">
-                        <c:v>4.5599999999999996</c:v>
-                      </c:pt>
-                      <c:pt idx="1" formatCode="General">
-                        <c:v>4.54</c:v>
-                      </c:pt>
-                      <c:pt idx="2" formatCode="General">
-                        <c:v>4.5199999999999996</c:v>
-                      </c:pt>
-                      <c:pt idx="3" formatCode="General">
-                        <c:v>4.5</c:v>
-                      </c:pt>
-                      <c:pt idx="4" formatCode="General">
-                        <c:v>4.49</c:v>
-                      </c:pt>
-                      <c:pt idx="5" formatCode="General">
-                        <c:v>4.49</c:v>
-                      </c:pt>
-                      <c:pt idx="6" formatCode="General">
-                        <c:v>4.4400000000000004</c:v>
-                      </c:pt>
-                      <c:pt idx="7" formatCode="General">
-                        <c:v>4.42</c:v>
-                      </c:pt>
-                      <c:pt idx="8" formatCode="General">
-                        <c:v>4.46</c:v>
-                      </c:pt>
-                      <c:pt idx="9" formatCode="General">
-                        <c:v>4.42</c:v>
-                      </c:pt>
-                      <c:pt idx="10" formatCode="General">
-                        <c:v>4.42</c:v>
-                      </c:pt>
-                      <c:pt idx="11" formatCode="General">
-                        <c:v>4.4400000000000004</c:v>
-                      </c:pt>
-                      <c:pt idx="12" formatCode="General">
-                        <c:v>4.47</c:v>
-                      </c:pt>
-                      <c:pt idx="13" formatCode="General">
-                        <c:v>4.29</c:v>
-                      </c:pt>
-                      <c:pt idx="14" formatCode="General">
-                        <c:v>4.3600000000000003</c:v>
+                      <c:ptCount val="17"/>
+                      <c:pt idx="0" formatCode="0.00">
+                        <c:v>0.25512798155620736</c:v>
+                      </c:pt>
+                      <c:pt idx="1" formatCode="0.00">
+                        <c:v>0.2541503130915318</c:v>
+                      </c:pt>
+                      <c:pt idx="2" formatCode="0.00">
+                        <c:v>0.25327727400311195</c:v>
+                      </c:pt>
+                      <c:pt idx="3" formatCode="0.00">
+                        <c:v>0.25240862980631523</c:v>
+                      </c:pt>
+                      <c:pt idx="4" formatCode="0.00">
+                        <c:v>0.25192844417416244</c:v>
+                      </c:pt>
+                      <c:pt idx="5" formatCode="0.00">
+                        <c:v>0.25183388649667288</c:v>
+                      </c:pt>
+                      <c:pt idx="6" formatCode="0.00">
+                        <c:v>0.24981482723255269</c:v>
+                      </c:pt>
+                      <c:pt idx="7" formatCode="0.00">
+                        <c:v>0.2489620323541514</c:v>
+                      </c:pt>
+                      <c:pt idx="8" formatCode="0.00">
+                        <c:v>0.2503975119963342</c:v>
+                      </c:pt>
+                      <c:pt idx="9" formatCode="0.00">
+                        <c:v>0.24880662534269438</c:v>
+                      </c:pt>
+                      <c:pt idx="10" formatCode="0.00">
+                        <c:v>0.24874052082979786</c:v>
+                      </c:pt>
+                      <c:pt idx="11" formatCode="0.00">
+                        <c:v>0.2493877007508046</c:v>
+                      </c:pt>
+                      <c:pt idx="12" formatCode="0.00">
+                        <c:v>0.25046605856839815</c:v>
+                      </c:pt>
+                      <c:pt idx="13" formatCode="0.00">
+                        <c:v>0.24361371243561997</c:v>
+                      </c:pt>
+                      <c:pt idx="14" formatCode="0.00">
+                        <c:v>0.24616698113392466</c:v>
+                      </c:pt>
+                      <c:pt idx="15" formatCode="0.00">
+                        <c:v>0.24798512728811881</c:v>
+                      </c:pt>
+                      <c:pt idx="16" formatCode="0.00">
+                        <c:v>0.24524172175943709</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1199,21 +1253,21 @@
             </c15:filteredLineSeries>
             <c15:filteredLineSeries>
               <c15:ser>
-                <c:idx val="1"/>
-                <c:order val="1"/>
+                <c:idx val="3"/>
+                <c:order val="3"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>GRAFICO!$A$5</c15:sqref>
+                          <c15:sqref>GRAFICO!$A$7</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
                       <c:ptCount val="1"/>
                       <c:pt idx="0">
-                        <c:v>COMPRA</c:v>
+                        <c:v>TITULO COMPRA</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -1221,7 +1275,7 @@
                 <c:spPr>
                   <a:ln w="28575" cap="rnd">
                     <a:solidFill>
-                      <a:schemeClr val="accent2"/>
+                      <a:schemeClr val="accent4"/>
                     </a:solidFill>
                     <a:round/>
                   </a:ln>
@@ -1232,11 +1286,11 @@
                   <c:size val="5"/>
                   <c:spPr>
                     <a:solidFill>
-                      <a:schemeClr val="accent2"/>
+                      <a:schemeClr val="accent4"/>
                     </a:solidFill>
                     <a:ln w="9525">
                       <a:solidFill>
-                        <a:schemeClr val="accent2"/>
+                        <a:schemeClr val="accent4"/>
                       </a:solidFill>
                     </a:ln>
                     <a:effectLst/>
@@ -1247,15 +1301,15 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$2:$AG$3</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$2:$AK$3</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$D$2:$D$3,GRAFICO!$F$2:$F$3,GRAFICO!$H$2:$H$3,GRAFICO!$J$2:$J$3,GRAFICO!$L$2:$L$3,GRAFICO!$N$2:$N$3,GRAFICO!$P$2:$P$3,GRAFICO!$R$2:$R$3,GRAFICO!$T$2:$T$3,GRAFICO!$V$2:$V$3,GRAFICO!$X$2:$X$3,GRAFICO!$Z$2:$Z$3,GRAFICO!$AB$2:$AB$3,GRAFICO!$AD$2:$AD$3,GRAFICO!$AF$2:$AF$3)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$D$2:$D$3,GRAFICO!$F$2:$F$3,GRAFICO!$H$2:$H$3,GRAFICO!$J$2:$J$3,GRAFICO!$L$2:$L$3,GRAFICO!$N$2:$N$3,GRAFICO!$P$2:$P$3,GRAFICO!$R$2:$R$3,GRAFICO!$T$2:$T$3,GRAFICO!$V$2:$V$3,GRAFICO!$X$2:$X$3,GRAFICO!$Z$2:$Z$3,GRAFICO!$AB$2:$AB$3,GRAFICO!$AD$2:$AD$3,GRAFICO!$AF$2:$AF$3,GRAFICO!$AH$2:$AH$3,GRAFICO!$AJ$2:$AJ$3)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:multiLvlStrCache>
-                      <c:ptCount val="15"/>
+                      <c:ptCount val="17"/>
                       <c:lvl>
                         <c:pt idx="0">
                           <c:v>02/05</c:v>
@@ -1301,6 +1355,12 @@
                         </c:pt>
                         <c:pt idx="14">
                           <c:v>22/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="15">
+                          <c:v>23/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="16">
+                          <c:v>24/mai</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
@@ -1347,6 +1407,12 @@
                           <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="14">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="15">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="16">
                           <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                       </c:lvl>
@@ -1358,60 +1424,66 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$5:$AG$5</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$7:$AK$7</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$D$5,GRAFICO!$F$5,GRAFICO!$H$5,GRAFICO!$J$5,GRAFICO!$L$5,GRAFICO!$N$5,GRAFICO!$P$5,GRAFICO!$R$5,GRAFICO!$T$5,GRAFICO!$V$5,GRAFICO!$X$5,GRAFICO!$Z$5,GRAFICO!$AB$5,GRAFICO!$AD$5,GRAFICO!$AF$5)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$D$7,GRAFICO!$F$7,GRAFICO!$H$7,GRAFICO!$J$7,GRAFICO!$L$7,GRAFICO!$N$7,GRAFICO!$P$7,GRAFICO!$R$7,GRAFICO!$T$7,GRAFICO!$V$7,GRAFICO!$X$7,GRAFICO!$Z$7,GRAFICO!$AB$7,GRAFICO!$AD$7,GRAFICO!$AF$7,GRAFICO!$AH$7,GRAFICO!$AJ$7)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>m/d/yyyy</c:formatCode>
-                      <c:ptCount val="15"/>
+                      <c:ptCount val="17"/>
                       <c:pt idx="0" formatCode="General">
-                        <c:v>4.4400000000000004</c:v>
-                      </c:pt>
-                      <c:pt idx="1" formatCode="General">
-                        <c:v>4.42</c:v>
-                      </c:pt>
-                      <c:pt idx="2" formatCode="General">
-                        <c:v>4.4000000000000004</c:v>
-                      </c:pt>
-                      <c:pt idx="3" formatCode="General">
-                        <c:v>4.38</c:v>
-                      </c:pt>
-                      <c:pt idx="4" formatCode="General">
-                        <c:v>4.37</c:v>
-                      </c:pt>
-                      <c:pt idx="5" formatCode="General">
-                        <c:v>4.37</c:v>
-                      </c:pt>
-                      <c:pt idx="6" formatCode="General">
-                        <c:v>4.32</c:v>
-                      </c:pt>
-                      <c:pt idx="7" formatCode="General">
-                        <c:v>4.3</c:v>
-                      </c:pt>
-                      <c:pt idx="8" formatCode="General">
-                        <c:v>4.34</c:v>
-                      </c:pt>
-                      <c:pt idx="9" formatCode="General">
-                        <c:v>4.3</c:v>
-                      </c:pt>
-                      <c:pt idx="10" formatCode="General">
-                        <c:v>4.3</c:v>
-                      </c:pt>
-                      <c:pt idx="11" formatCode="General">
-                        <c:v>4.32</c:v>
-                      </c:pt>
-                      <c:pt idx="12" formatCode="General">
-                        <c:v>4.3499999999999996</c:v>
-                      </c:pt>
-                      <c:pt idx="13" formatCode="General">
-                        <c:v>4.41</c:v>
-                      </c:pt>
-                      <c:pt idx="14" formatCode="General">
-                        <c:v>4.24</c:v>
+                        <c:v>0.25</c:v>
+                      </c:pt>
+                      <c:pt idx="1" formatCode="0.00">
+                        <c:v>0.24952682055163874</c:v>
+                      </c:pt>
+                      <c:pt idx="2" formatCode="0.00">
+                        <c:v>0.24867137929272118</c:v>
+                      </c:pt>
+                      <c:pt idx="3" formatCode="0.00">
+                        <c:v>0.24781873222465564</c:v>
+                      </c:pt>
+                      <c:pt idx="4" formatCode="0.00">
+                        <c:v>0.2473482365854324</c:v>
+                      </c:pt>
+                      <c:pt idx="5" formatCode="0.00">
+                        <c:v>0.24725556664045298</c:v>
+                      </c:pt>
+                      <c:pt idx="6" formatCode="0.00">
+                        <c:v>0.24527160486979319</c:v>
+                      </c:pt>
+                      <c:pt idx="7" formatCode="0.00">
+                        <c:v>0.24443613706365483</c:v>
+                      </c:pt>
+                      <c:pt idx="8" formatCode="0.00">
+                        <c:v>0.24584827750825125</c:v>
+                      </c:pt>
+                      <c:pt idx="9" formatCode="0.00">
+                        <c:v>0.24428484495287314</c:v>
+                      </c:pt>
+                      <c:pt idx="10" formatCode="0.00">
+                        <c:v>0.2442211210488876</c:v>
+                      </c:pt>
+                      <c:pt idx="11" formatCode="0.00">
+                        <c:v>0.24485986006750585</c:v>
+                      </c:pt>
+                      <c:pt idx="12" formatCode="0.00">
+                        <c:v>0.24592036452861396</c:v>
+                      </c:pt>
+                      <c:pt idx="13" formatCode="0.00">
+                        <c:v>0.248118098462867</c:v>
+                      </c:pt>
+                      <c:pt idx="14" formatCode="0.00">
+                        <c:v>0.24169624280267191</c:v>
+                      </c:pt>
+                      <c:pt idx="15" formatCode="0.00">
+                        <c:v>0.24348552416080169</c:v>
+                      </c:pt>
+                      <c:pt idx="16" formatCode="0.00">
+                        <c:v>0.24078982225923135</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1423,7 +1495,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-364703168"/>
+        <c:axId val="-545832192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1466,7 +1538,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-364698816"/>
+        <c:crossAx val="-545829472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1474,7 +1546,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-364698816"/>
+        <c:axId val="-545829472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1525,7 +1597,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-364703168"/>
+        <c:crossAx val="-545832192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1730,13 +1802,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$2:$AC$3</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$2:$AK$3</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$E$2:$E$3,GRAFICO!$G$2:$G$3,GRAFICO!$I$2:$I$3,GRAFICO!$K$2:$K$3,GRAFICO!$M$2:$M$3,GRAFICO!$O$2:$O$3,GRAFICO!$Q$2:$Q$3,GRAFICO!$S$2:$S$3,GRAFICO!$U$2:$U$3,GRAFICO!$W$2:$W$3,GRAFICO!$Y$2:$Y$3,GRAFICO!$AA$2:$AA$3,GRAFICO!$AC$2:$AC$3)</c:f>
+              <c:f>(GRAFICO!$E$2:$E$3,GRAFICO!$G$2:$G$3,GRAFICO!$I$2:$I$3,GRAFICO!$K$2:$K$3,GRAFICO!$M$2:$M$3,GRAFICO!$O$2:$O$3,GRAFICO!$Q$2:$Q$3,GRAFICO!$S$2:$S$3,GRAFICO!$U$2:$U$3,GRAFICO!$W$2:$W$3,GRAFICO!$Y$2:$Y$3,GRAFICO!$AA$2:$AA$3,GRAFICO!$AC$2:$AC$3,GRAFICO!$AE$2:$AE$3,GRAFICO!$AG$2:$AG$3,GRAFICO!$AI$2:$AI$3,GRAFICO!$AK$2:$AK$3)</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="17"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>02/05</c:v>
@@ -1776,6 +1848,18 @@
                   </c:pt>
                   <c:pt idx="12">
                     <c:v>20/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>21/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>22/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>23/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>24/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -1816,6 +1900,18 @@
                     <c:v>Preço Unitário</c:v>
                   </c:pt>
                   <c:pt idx="12">
+                    <c:v>Preço Unitário</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>Preço Unitário</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>Preço Unitário</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>Preço Unitário</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
                     <c:v>Preço Unitário</c:v>
                   </c:pt>
                 </c:lvl>
@@ -1827,14 +1923,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$4:$AC$4</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$4:$AK$4</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$E$4,GRAFICO!$G$4,GRAFICO!$I$4,GRAFICO!$K$4,GRAFICO!$M$4,GRAFICO!$O$4,GRAFICO!$Q$4,GRAFICO!$S$4,GRAFICO!$U$4,GRAFICO!$W$4,GRAFICO!$Y$4,GRAFICO!$AA$4,GRAFICO!$AC$4)</c:f>
+              <c:f>(GRAFICO!$E$4,GRAFICO!$G$4,GRAFICO!$I$4,GRAFICO!$K$4,GRAFICO!$M$4,GRAFICO!$O$4,GRAFICO!$Q$4,GRAFICO!$S$4,GRAFICO!$U$4,GRAFICO!$W$4,GRAFICO!$Y$4,GRAFICO!$AA$4,GRAFICO!$AC$4,GRAFICO!$AE$4,GRAFICO!$AG$4,GRAFICO!$AI$4,GRAFICO!$AK$4)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>1577.93</c:v>
                 </c:pt>
@@ -1873,6 +1969,18 @@
                 </c:pt>
                 <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>1607.3</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1652.51</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1635.37</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1623.38</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1641.54</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1922,13 +2030,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$2:$AC$3</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$2:$AK$3</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$E$2:$E$3,GRAFICO!$G$2:$G$3,GRAFICO!$I$2:$I$3,GRAFICO!$K$2:$K$3,GRAFICO!$M$2:$M$3,GRAFICO!$O$2:$O$3,GRAFICO!$Q$2:$Q$3,GRAFICO!$S$2:$S$3,GRAFICO!$U$2:$U$3,GRAFICO!$W$2:$W$3,GRAFICO!$Y$2:$Y$3,GRAFICO!$AA$2:$AA$3,GRAFICO!$AC$2:$AC$3)</c:f>
+              <c:f>(GRAFICO!$E$2:$E$3,GRAFICO!$G$2:$G$3,GRAFICO!$I$2:$I$3,GRAFICO!$K$2:$K$3,GRAFICO!$M$2:$M$3,GRAFICO!$O$2:$O$3,GRAFICO!$Q$2:$Q$3,GRAFICO!$S$2:$S$3,GRAFICO!$U$2:$U$3,GRAFICO!$W$2:$W$3,GRAFICO!$Y$2:$Y$3,GRAFICO!$AA$2:$AA$3,GRAFICO!$AC$2:$AC$3,GRAFICO!$AE$2:$AE$3,GRAFICO!$AG$2:$AG$3,GRAFICO!$AI$2:$AI$3,GRAFICO!$AK$2:$AK$3)</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="17"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>02/05</c:v>
@@ -1968,6 +2076,18 @@
                   </c:pt>
                   <c:pt idx="12">
                     <c:v>20/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>21/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>22/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>23/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>24/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -2008,6 +2128,18 @@
                     <c:v>Preço Unitário</c:v>
                   </c:pt>
                   <c:pt idx="12">
+                    <c:v>Preço Unitário</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>Preço Unitário</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>Preço Unitário</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>Preço Unitário</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
                     <c:v>Preço Unitário</c:v>
                   </c:pt>
                 </c:lvl>
@@ -2019,14 +2151,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$5:$AC$5</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$5:$AK$5</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$E$5,GRAFICO!$G$5,GRAFICO!$I$5,GRAFICO!$K$5,GRAFICO!$M$5,GRAFICO!$O$5,GRAFICO!$Q$5,GRAFICO!$S$5,GRAFICO!$U$5,GRAFICO!$W$5,GRAFICO!$Y$5,GRAFICO!$AA$5,GRAFICO!$AC$5)</c:f>
+              <c:f>(GRAFICO!$E$5,GRAFICO!$G$5,GRAFICO!$I$5,GRAFICO!$K$5,GRAFICO!$M$5,GRAFICO!$O$5,GRAFICO!$Q$5,GRAFICO!$S$5,GRAFICO!$U$5,GRAFICO!$W$5,GRAFICO!$Y$5,GRAFICO!$AA$5,GRAFICO!$AC$5,GRAFICO!$AE$5,GRAFICO!$AG$5,GRAFICO!$AI$5,GRAFICO!$AK$5)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>1607.16</c:v>
                 </c:pt>
@@ -2065,6 +2197,18 @@
                 </c:pt>
                 <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                   <c:v>1637.01</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1622.51</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1665.62</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1653.38</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                  <c:v>1671.89</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2081,11 +2225,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-364695008"/>
-        <c:axId val="-364697184"/>
+        <c:axId val="-273373200"/>
+        <c:axId val="-273375920"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-364695008"/>
+        <c:axId val="-273373200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2128,7 +2272,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-364697184"/>
+        <c:crossAx val="-273375920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2136,7 +2280,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-364697184"/>
+        <c:axId val="-273375920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2187,7 +2331,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-364695008"/>
+        <c:crossAx val="-273373200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2362,13 +2506,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$2:$AG$3</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$2:$AK$3</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$E$2:$E$3,GRAFICO!$G$2:$G$3,GRAFICO!$I$2:$I$3,GRAFICO!$K$2:$K$3,GRAFICO!$M$2:$M$3,GRAFICO!$O$2:$O$3,GRAFICO!$Q$2:$Q$3,GRAFICO!$S$2:$S$3,GRAFICO!$U$2:$U$3,GRAFICO!$W$2:$W$3,GRAFICO!$Y$2:$Y$3,GRAFICO!$AA$2:$AA$3,GRAFICO!$AC$2:$AC$3,GRAFICO!$AE$2:$AE$3,GRAFICO!$AG$2:$AG$3)</c:f>
+              <c:f>(GRAFICO!$D$2:$D$3,GRAFICO!$F$2:$F$3,GRAFICO!$H$2:$H$3,GRAFICO!$J$2:$J$3,GRAFICO!$L$2:$L$3,GRAFICO!$N$2:$N$3,GRAFICO!$P$2:$P$3,GRAFICO!$R$2:$R$3,GRAFICO!$T$2:$T$3,GRAFICO!$V$2:$V$3,GRAFICO!$X$2:$X$3,GRAFICO!$Z$2:$Z$3,GRAFICO!$AB$2:$AB$3,GRAFICO!$AD$2:$AD$3,GRAFICO!$AF$2:$AF$3,GRAFICO!$AH$2:$AH$3,GRAFICO!$AJ$2:$AJ$3)</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="15"/>
+                <c:ptCount val="17"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>02/05</c:v>
@@ -2415,52 +2559,64 @@
                   <c:pt idx="14">
                     <c:v>22/mai</c:v>
                   </c:pt>
+                  <c:pt idx="15">
+                    <c:v>23/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>24/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>Preço Unitário</c:v>
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>Preço Unitário</c:v>
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>Preço Unitário</c:v>
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>Preço Unitário</c:v>
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>Preço Unitário</c:v>
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>Preço Unitário</c:v>
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>Preço Unitário</c:v>
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>Preço Unitário</c:v>
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>Preço Unitário</c:v>
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>Preço Unitário</c:v>
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>Preço Unitário</c:v>
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>Preço Unitário</c:v>
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>Preço Unitário</c:v>
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>Preço Unitário</c:v>
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>Preço Unitário</c:v>
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -2471,58 +2627,64 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$6:$AG$6</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$6:$AK$6</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$E$6,GRAFICO!$G$6,GRAFICO!$I$6,GRAFICO!$K$6,GRAFICO!$M$6,GRAFICO!$O$6,GRAFICO!$Q$6,GRAFICO!$S$6,GRAFICO!$U$6,GRAFICO!$W$6,GRAFICO!$Y$6,GRAFICO!$AA$6,GRAFICO!$AC$6,GRAFICO!$AE$6,GRAFICO!$AG$6)</c:f>
+              <c:f>(GRAFICO!$D$6,GRAFICO!$F$6,GRAFICO!$H$6,GRAFICO!$J$6,GRAFICO!$L$6,GRAFICO!$N$6,GRAFICO!$P$6,GRAFICO!$R$6,GRAFICO!$T$6,GRAFICO!$V$6,GRAFICO!$X$6,GRAFICO!$Z$6,GRAFICO!$AB$6,GRAFICO!$AD$6,GRAFICO!$AF$6,GRAFICO!$AH$6,GRAFICO!$AJ$6)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="15"/>
-                <c:pt idx="0" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>5.0196230136986299E-2</c:v>
-                </c:pt>
-                <c:pt idx="1" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.10017230136986301</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.14992821369863013</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.19946396712328768</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.24888964109589043</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.29831531506849318</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.34719059178082196</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.39584570958904114</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.4449411452054795</c:v>
-                </c:pt>
-                <c:pt idx="9" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.49359626301369869</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.54225138082191782</c:v>
-                </c:pt>
-                <c:pt idx="11" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.59112665753424665</c:v>
-                </c:pt>
-                <c:pt idx="12" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.64033217260273978</c:v>
-                </c:pt>
-                <c:pt idx="13" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.68755625753424665</c:v>
-                </c:pt>
-                <c:pt idx="14" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.73555089863013712</c:v>
+                <c:ptCount val="17"/>
+                <c:pt idx="0" formatCode="0.00">
+                  <c:v>0.25512798155620736</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="0.00">
+                  <c:v>0.2541503130915318</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.00">
+                  <c:v>0.25327727400311195</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00">
+                  <c:v>0.25240862980631523</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00">
+                  <c:v>0.25192844417416244</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00">
+                  <c:v>0.25183388649667288</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.00">
+                  <c:v>0.24981482723255269</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.00">
+                  <c:v>0.2489620323541514</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.00">
+                  <c:v>0.2503975119963342</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.00">
+                  <c:v>0.24880662534269438</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="0.00">
+                  <c:v>0.24874052082979786</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="0.00">
+                  <c:v>0.2493877007508046</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="0.00">
+                  <c:v>0.25046605856839815</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="0.00">
+                  <c:v>0.24361371243561997</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="0.00">
+                  <c:v>0.24616698113392466</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="0.00">
+                  <c:v>0.24798512728811881</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="0.00">
+                  <c:v>0.24524172175943709</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2572,13 +2734,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$2:$AG$3</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$2:$AK$3</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$E$2:$E$3,GRAFICO!$G$2:$G$3,GRAFICO!$I$2:$I$3,GRAFICO!$K$2:$K$3,GRAFICO!$M$2:$M$3,GRAFICO!$O$2:$O$3,GRAFICO!$Q$2:$Q$3,GRAFICO!$S$2:$S$3,GRAFICO!$U$2:$U$3,GRAFICO!$W$2:$W$3,GRAFICO!$Y$2:$Y$3,GRAFICO!$AA$2:$AA$3,GRAFICO!$AC$2:$AC$3,GRAFICO!$AE$2:$AE$3,GRAFICO!$AG$2:$AG$3)</c:f>
+              <c:f>(GRAFICO!$D$2:$D$3,GRAFICO!$F$2:$F$3,GRAFICO!$H$2:$H$3,GRAFICO!$J$2:$J$3,GRAFICO!$L$2:$L$3,GRAFICO!$N$2:$N$3,GRAFICO!$P$2:$P$3,GRAFICO!$R$2:$R$3,GRAFICO!$T$2:$T$3,GRAFICO!$V$2:$V$3,GRAFICO!$X$2:$X$3,GRAFICO!$Z$2:$Z$3,GRAFICO!$AB$2:$AB$3,GRAFICO!$AD$2:$AD$3,GRAFICO!$AF$2:$AF$3,GRAFICO!$AH$2:$AH$3,GRAFICO!$AJ$2:$AJ$3)</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="15"/>
+                <c:ptCount val="17"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>02/05</c:v>
@@ -2625,52 +2787,64 @@
                   <c:pt idx="14">
                     <c:v>22/mai</c:v>
                   </c:pt>
+                  <c:pt idx="15">
+                    <c:v>23/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>24/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>Preço Unitário</c:v>
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>Preço Unitário</c:v>
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>Preço Unitário</c:v>
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>Preço Unitário</c:v>
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>Preço Unitário</c:v>
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>Preço Unitário</c:v>
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>Preço Unitário</c:v>
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>Preço Unitário</c:v>
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>Preço Unitário</c:v>
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>Preço Unitário</c:v>
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>Preço Unitário</c:v>
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>Preço Unitário</c:v>
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>Preço Unitário</c:v>
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>Preço Unitário</c:v>
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>Preço Unitário</c:v>
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>Taxa de Rendimento (% a.a.)</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -2681,58 +2855,64 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$7:$AG$7</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$7:$AK$7</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$E$7,GRAFICO!$G$7,GRAFICO!$I$7,GRAFICO!$K$7,GRAFICO!$M$7,GRAFICO!$O$7,GRAFICO!$Q$7,GRAFICO!$S$7,GRAFICO!$U$7,GRAFICO!$W$7,GRAFICO!$Y$7,GRAFICO!$AA$7,GRAFICO!$AC$7,GRAFICO!$AE$7,GRAFICO!$AG$7)</c:f>
+              <c:f>(GRAFICO!$D$7,GRAFICO!$F$7,GRAFICO!$H$7,GRAFICO!$J$7,GRAFICO!$L$7,GRAFICO!$N$7,GRAFICO!$P$7,GRAFICO!$R$7,GRAFICO!$T$7,GRAFICO!$V$7,GRAFICO!$X$7,GRAFICO!$Z$7,GRAFICO!$AB$7,GRAFICO!$AD$7,GRAFICO!$AF$7,GRAFICO!$AH$7,GRAFICO!$AJ$7)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="15"/>
-                <c:pt idx="0" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>4.8875276712328775E-2</c:v>
-                </c:pt>
-                <c:pt idx="1" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>9.7530394520547958E-2</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.14596535342465755</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.19418015342465755</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.24228487397260276</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.29038959452054797</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.3379439178082192</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.38527808219178084</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.43305256438356166</c:v>
-                </c:pt>
-                <c:pt idx="9" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.48038672876712329</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.52772089315068493</c:v>
-                </c:pt>
-                <c:pt idx="11" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.57527521643835622</c:v>
-                </c:pt>
-                <c:pt idx="12" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.62315977808219181</c:v>
-                </c:pt>
-                <c:pt idx="13" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.67170481643835622</c:v>
-                </c:pt>
-                <c:pt idx="14" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
-                  <c:v>0.71837850410958914</c:v>
+                <c:ptCount val="17"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="0.00">
+                  <c:v>0.24952682055163874</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.00">
+                  <c:v>0.24867137929272118</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00">
+                  <c:v>0.24781873222465564</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00">
+                  <c:v>0.2473482365854324</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00">
+                  <c:v>0.24725556664045298</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.00">
+                  <c:v>0.24527160486979319</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.00">
+                  <c:v>0.24443613706365483</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.00">
+                  <c:v>0.24584827750825125</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.00">
+                  <c:v>0.24428484495287314</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="0.00">
+                  <c:v>0.2442211210488876</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="0.00">
+                  <c:v>0.24485986006750585</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="0.00">
+                  <c:v>0.24592036452861396</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="0.00">
+                  <c:v>0.248118098462867</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="0.00">
+                  <c:v>0.24169624280267191</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="0.00">
+                  <c:v>0.24348552416080169</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="0.00">
+                  <c:v>0.24078982225923135</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2749,8 +2929,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-364697728"/>
-        <c:axId val="-364702624"/>
+        <c:axId val="-273371024"/>
+        <c:axId val="-273380272"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -2803,15 +2983,15 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$2:$AG$3</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$2:$AK$3</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$E$2:$E$3,GRAFICO!$G$2:$G$3,GRAFICO!$I$2:$I$3,GRAFICO!$K$2:$K$3,GRAFICO!$M$2:$M$3,GRAFICO!$O$2:$O$3,GRAFICO!$Q$2:$Q$3,GRAFICO!$S$2:$S$3,GRAFICO!$U$2:$U$3,GRAFICO!$W$2:$W$3,GRAFICO!$Y$2:$Y$3,GRAFICO!$AA$2:$AA$3,GRAFICO!$AC$2:$AC$3,GRAFICO!$AE$2:$AE$3,GRAFICO!$AG$2:$AG$3)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$D$2:$D$3,GRAFICO!$F$2:$F$3,GRAFICO!$H$2:$H$3,GRAFICO!$J$2:$J$3,GRAFICO!$L$2:$L$3,GRAFICO!$N$2:$N$3,GRAFICO!$P$2:$P$3,GRAFICO!$R$2:$R$3,GRAFICO!$T$2:$T$3,GRAFICO!$V$2:$V$3,GRAFICO!$X$2:$X$3,GRAFICO!$Z$2:$Z$3,GRAFICO!$AB$2:$AB$3,GRAFICO!$AD$2:$AD$3,GRAFICO!$AF$2:$AF$3,GRAFICO!$AH$2:$AH$3,GRAFICO!$AJ$2:$AJ$3)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:multiLvlStrCache>
-                      <c:ptCount val="15"/>
+                      <c:ptCount val="17"/>
                       <c:lvl>
                         <c:pt idx="0">
                           <c:v>02/05</c:v>
@@ -2858,52 +3038,64 @@
                         <c:pt idx="14">
                           <c:v>22/mai</c:v>
                         </c:pt>
+                        <c:pt idx="15">
+                          <c:v>23/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="16">
+                          <c:v>24/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
-                          <c:v>Preço Unitário</c:v>
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="1">
-                          <c:v>Preço Unitário</c:v>
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="2">
-                          <c:v>Preço Unitário</c:v>
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="3">
-                          <c:v>Preço Unitário</c:v>
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="4">
-                          <c:v>Preço Unitário</c:v>
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="5">
-                          <c:v>Preço Unitário</c:v>
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="6">
-                          <c:v>Preço Unitário</c:v>
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="7">
-                          <c:v>Preço Unitário</c:v>
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="8">
-                          <c:v>Preço Unitário</c:v>
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="9">
-                          <c:v>Preço Unitário</c:v>
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="10">
-                          <c:v>Preço Unitário</c:v>
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="11">
-                          <c:v>Preço Unitário</c:v>
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="12">
-                          <c:v>Preço Unitário</c:v>
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="13">
-                          <c:v>Preço Unitário</c:v>
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="14">
-                          <c:v>Preço Unitário</c:v>
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="15">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="16">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                       </c:lvl>
                     </c:multiLvlStrCache>
@@ -2914,60 +3106,66 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$4:$AG$4</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$4:$AK$4</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$E$4,GRAFICO!$G$4,GRAFICO!$I$4,GRAFICO!$K$4,GRAFICO!$M$4,GRAFICO!$O$4,GRAFICO!$Q$4,GRAFICO!$S$4,GRAFICO!$U$4,GRAFICO!$W$4,GRAFICO!$Y$4,GRAFICO!$AA$4,GRAFICO!$AC$4,GRAFICO!$AE$4,GRAFICO!$AG$4)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$D$4,GRAFICO!$F$4,GRAFICO!$H$4,GRAFICO!$J$4,GRAFICO!$L$4,GRAFICO!$N$4,GRAFICO!$P$4,GRAFICO!$R$4,GRAFICO!$T$4,GRAFICO!$V$4,GRAFICO!$X$4,GRAFICO!$Z$4,GRAFICO!$AB$4,GRAFICO!$AD$4,GRAFICO!$AF$4,GRAFICO!$AH$4,GRAFICO!$AJ$4)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>m/d/yyyy</c:formatCode>
-                      <c:ptCount val="15"/>
-                      <c:pt idx="0" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
-                        <c:v>1577.93</c:v>
-                      </c:pt>
-                      <c:pt idx="1" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
-                        <c:v>1584</c:v>
-                      </c:pt>
-                      <c:pt idx="2" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
-                        <c:v>1589.46</c:v>
-                      </c:pt>
-                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
-                        <c:v>1594.93</c:v>
-                      </c:pt>
-                      <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
-                        <c:v>1597.97</c:v>
-                      </c:pt>
-                      <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
-                        <c:v>1598.57</c:v>
-                      </c:pt>
-                      <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
-                        <c:v>1611.49</c:v>
-                      </c:pt>
-                      <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
-                        <c:v>1617.01</c:v>
-                      </c:pt>
-                      <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
-                        <c:v>1607.74</c:v>
-                      </c:pt>
-                      <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
-                        <c:v>1618.02</c:v>
-                      </c:pt>
-                      <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
-                        <c:v>1618.45</c:v>
-                      </c:pt>
-                      <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
-                        <c:v>1614.25</c:v>
-                      </c:pt>
-                      <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
-                        <c:v>1607.3</c:v>
-                      </c:pt>
-                      <c:pt idx="13" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
-                        <c:v>1652.51</c:v>
-                      </c:pt>
-                      <c:pt idx="14" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
-                        <c:v>1635.37</c:v>
+                      <c:ptCount val="17"/>
+                      <c:pt idx="0" formatCode="General">
+                        <c:v>4.5599999999999996</c:v>
+                      </c:pt>
+                      <c:pt idx="1" formatCode="General">
+                        <c:v>4.54</c:v>
+                      </c:pt>
+                      <c:pt idx="2" formatCode="General">
+                        <c:v>4.5199999999999996</c:v>
+                      </c:pt>
+                      <c:pt idx="3" formatCode="General">
+                        <c:v>4.5</c:v>
+                      </c:pt>
+                      <c:pt idx="4" formatCode="General">
+                        <c:v>4.49</c:v>
+                      </c:pt>
+                      <c:pt idx="5" formatCode="General">
+                        <c:v>4.49</c:v>
+                      </c:pt>
+                      <c:pt idx="6" formatCode="General">
+                        <c:v>4.4400000000000004</c:v>
+                      </c:pt>
+                      <c:pt idx="7" formatCode="General">
+                        <c:v>4.42</c:v>
+                      </c:pt>
+                      <c:pt idx="8" formatCode="General">
+                        <c:v>4.46</c:v>
+                      </c:pt>
+                      <c:pt idx="9" formatCode="General">
+                        <c:v>4.42</c:v>
+                      </c:pt>
+                      <c:pt idx="10" formatCode="General">
+                        <c:v>4.42</c:v>
+                      </c:pt>
+                      <c:pt idx="11" formatCode="General">
+                        <c:v>4.4400000000000004</c:v>
+                      </c:pt>
+                      <c:pt idx="12" formatCode="General">
+                        <c:v>4.47</c:v>
+                      </c:pt>
+                      <c:pt idx="13" formatCode="General">
+                        <c:v>4.29</c:v>
+                      </c:pt>
+                      <c:pt idx="14" formatCode="General">
+                        <c:v>4.3600000000000003</c:v>
+                      </c:pt>
+                      <c:pt idx="15" formatCode="General">
+                        <c:v>4.41</c:v>
+                      </c:pt>
+                      <c:pt idx="16" formatCode="General">
+                        <c:v>4.34</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2981,7 +3179,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>GRAFICO!$A$5</c15:sqref>
@@ -3025,15 +3223,15 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$2:$AG$3</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$2:$AK$3</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$E$2:$E$3,GRAFICO!$G$2:$G$3,GRAFICO!$I$2:$I$3,GRAFICO!$K$2:$K$3,GRAFICO!$M$2:$M$3,GRAFICO!$O$2:$O$3,GRAFICO!$Q$2:$Q$3,GRAFICO!$S$2:$S$3,GRAFICO!$U$2:$U$3,GRAFICO!$W$2:$W$3,GRAFICO!$Y$2:$Y$3,GRAFICO!$AA$2:$AA$3,GRAFICO!$AC$2:$AC$3,GRAFICO!$AE$2:$AE$3,GRAFICO!$AG$2:$AG$3)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$D$2:$D$3,GRAFICO!$F$2:$F$3,GRAFICO!$H$2:$H$3,GRAFICO!$J$2:$J$3,GRAFICO!$L$2:$L$3,GRAFICO!$N$2:$N$3,GRAFICO!$P$2:$P$3,GRAFICO!$R$2:$R$3,GRAFICO!$T$2:$T$3,GRAFICO!$V$2:$V$3,GRAFICO!$X$2:$X$3,GRAFICO!$Z$2:$Z$3,GRAFICO!$AB$2:$AB$3,GRAFICO!$AD$2:$AD$3,GRAFICO!$AF$2:$AF$3,GRAFICO!$AH$2:$AH$3,GRAFICO!$AJ$2:$AJ$3)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:multiLvlStrCache>
-                      <c:ptCount val="15"/>
+                      <c:ptCount val="17"/>
                       <c:lvl>
                         <c:pt idx="0">
                           <c:v>02/05</c:v>
@@ -3080,52 +3278,64 @@
                         <c:pt idx="14">
                           <c:v>22/mai</c:v>
                         </c:pt>
+                        <c:pt idx="15">
+                          <c:v>23/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="16">
+                          <c:v>24/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
-                          <c:v>Preço Unitário</c:v>
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="1">
-                          <c:v>Preço Unitário</c:v>
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="2">
-                          <c:v>Preço Unitário</c:v>
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="3">
-                          <c:v>Preço Unitário</c:v>
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="4">
-                          <c:v>Preço Unitário</c:v>
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="5">
-                          <c:v>Preço Unitário</c:v>
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="6">
-                          <c:v>Preço Unitário</c:v>
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="7">
-                          <c:v>Preço Unitário</c:v>
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="8">
-                          <c:v>Preço Unitário</c:v>
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="9">
-                          <c:v>Preço Unitário</c:v>
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="10">
-                          <c:v>Preço Unitário</c:v>
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="11">
-                          <c:v>Preço Unitário</c:v>
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="12">
-                          <c:v>Preço Unitário</c:v>
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="13">
-                          <c:v>Preço Unitário</c:v>
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                         <c:pt idx="14">
-                          <c:v>Preço Unitário</c:v>
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="15">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
+                        </c:pt>
+                        <c:pt idx="16">
+                          <c:v>Taxa de Rendimento (% a.a.)</c:v>
                         </c:pt>
                       </c:lvl>
                     </c:multiLvlStrCache>
@@ -3136,60 +3346,66 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$5:$AG$5</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$5:$AK$5</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$E$5,GRAFICO!$G$5,GRAFICO!$I$5,GRAFICO!$K$5,GRAFICO!$M$5,GRAFICO!$O$5,GRAFICO!$Q$5,GRAFICO!$S$5,GRAFICO!$U$5,GRAFICO!$W$5,GRAFICO!$Y$5,GRAFICO!$AA$5,GRAFICO!$AC$5,GRAFICO!$AE$5,GRAFICO!$AG$5)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$D$5,GRAFICO!$F$5,GRAFICO!$H$5,GRAFICO!$J$5,GRAFICO!$L$5,GRAFICO!$N$5,GRAFICO!$P$5,GRAFICO!$R$5,GRAFICO!$T$5,GRAFICO!$V$5,GRAFICO!$X$5,GRAFICO!$Z$5,GRAFICO!$AB$5,GRAFICO!$AD$5,GRAFICO!$AF$5,GRAFICO!$AH$5,GRAFICO!$AJ$5)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>m/d/yyyy</c:formatCode>
-                      <c:ptCount val="15"/>
-                      <c:pt idx="0" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
-                        <c:v>1607.16</c:v>
-                      </c:pt>
-                      <c:pt idx="1" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
-                        <c:v>1613.35</c:v>
-                      </c:pt>
-                      <c:pt idx="2" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
-                        <c:v>1618.9</c:v>
-                      </c:pt>
-                      <c:pt idx="3" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
-                        <c:v>1624.47</c:v>
-                      </c:pt>
-                      <c:pt idx="4" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
-                        <c:v>1627.56</c:v>
-                      </c:pt>
-                      <c:pt idx="5" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
-                        <c:v>1628.17</c:v>
-                      </c:pt>
-                      <c:pt idx="6" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
-                        <c:v>1641.34</c:v>
-                      </c:pt>
-                      <c:pt idx="7" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
-                        <c:v>1646.95</c:v>
-                      </c:pt>
-                      <c:pt idx="8" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
-                        <c:v>1637.49</c:v>
-                      </c:pt>
-                      <c:pt idx="9" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
-                        <c:v>1647.97</c:v>
-                      </c:pt>
-                      <c:pt idx="10" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
-                        <c:v>1648.4</c:v>
-                      </c:pt>
-                      <c:pt idx="11" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
-                        <c:v>1644.1</c:v>
-                      </c:pt>
-                      <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
-                        <c:v>1637.01</c:v>
-                      </c:pt>
-                      <c:pt idx="13" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
-                        <c:v>1622.51</c:v>
-                      </c:pt>
-                      <c:pt idx="14" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
-                        <c:v>1665.62</c:v>
+                      <c:ptCount val="17"/>
+                      <c:pt idx="0" formatCode="General">
+                        <c:v>4.4400000000000004</c:v>
+                      </c:pt>
+                      <c:pt idx="1" formatCode="General">
+                        <c:v>4.42</c:v>
+                      </c:pt>
+                      <c:pt idx="2" formatCode="General">
+                        <c:v>4.4000000000000004</c:v>
+                      </c:pt>
+                      <c:pt idx="3" formatCode="General">
+                        <c:v>4.38</c:v>
+                      </c:pt>
+                      <c:pt idx="4" formatCode="General">
+                        <c:v>4.37</c:v>
+                      </c:pt>
+                      <c:pt idx="5" formatCode="General">
+                        <c:v>4.37</c:v>
+                      </c:pt>
+                      <c:pt idx="6" formatCode="General">
+                        <c:v>4.32</c:v>
+                      </c:pt>
+                      <c:pt idx="7" formatCode="General">
+                        <c:v>4.3</c:v>
+                      </c:pt>
+                      <c:pt idx="8" formatCode="General">
+                        <c:v>4.34</c:v>
+                      </c:pt>
+                      <c:pt idx="9" formatCode="General">
+                        <c:v>4.3</c:v>
+                      </c:pt>
+                      <c:pt idx="10" formatCode="General">
+                        <c:v>4.3</c:v>
+                      </c:pt>
+                      <c:pt idx="11" formatCode="General">
+                        <c:v>4.32</c:v>
+                      </c:pt>
+                      <c:pt idx="12" formatCode="General">
+                        <c:v>4.3499999999999996</c:v>
+                      </c:pt>
+                      <c:pt idx="13" formatCode="General">
+                        <c:v>4.41</c:v>
+                      </c:pt>
+                      <c:pt idx="14" formatCode="General">
+                        <c:v>4.24</c:v>
+                      </c:pt>
+                      <c:pt idx="15" formatCode="General">
+                        <c:v>4.29</c:v>
+                      </c:pt>
+                      <c:pt idx="16" formatCode="General">
+                        <c:v>4.22</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3201,7 +3417,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-364697728"/>
+        <c:axId val="-273371024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3244,7 +3460,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-364702624"/>
+        <c:crossAx val="-273380272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3252,7 +3468,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-364702624"/>
+        <c:axId val="-273380272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3272,7 +3488,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="&quot;R$&quot;#,##0.00" sourceLinked="0"/>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3303,7 +3519,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-364697728"/>
+        <c:crossAx val="-273371024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3399,6 +3615,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3477,13 +3694,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$2:$AC$3</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$2:$AK$3</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$E$2:$E$3,GRAFICO!$G$2:$G$3,GRAFICO!$I$2:$I$3,GRAFICO!$K$2:$K$3,GRAFICO!$M$2:$M$3,GRAFICO!$O$2:$O$3,GRAFICO!$Q$2:$Q$3,GRAFICO!$S$2:$S$3,GRAFICO!$U$2:$U$3,GRAFICO!$W$2:$W$3,GRAFICO!$Y$2:$Y$3,GRAFICO!$AA$2:$AA$3,GRAFICO!$AC$2:$AC$3)</c:f>
+              <c:f>(GRAFICO!$E$2:$E$3,GRAFICO!$G$2:$G$3,GRAFICO!$I$2:$I$3,GRAFICO!$K$2:$K$3,GRAFICO!$M$2:$M$3,GRAFICO!$O$2:$O$3,GRAFICO!$Q$2:$Q$3,GRAFICO!$S$2:$S$3,GRAFICO!$U$2:$U$3,GRAFICO!$W$2:$W$3,GRAFICO!$Y$2:$Y$3,GRAFICO!$AA$2:$AA$3,GRAFICO!$AC$2:$AC$3,GRAFICO!$AE$2:$AE$3,GRAFICO!$AG$2:$AG$3,GRAFICO!$AI$2:$AI$3,GRAFICO!$AK$2:$AK$3)</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="17"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>02/05</c:v>
@@ -3523,6 +3740,18 @@
                   </c:pt>
                   <c:pt idx="12">
                     <c:v>20/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>21/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>22/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>23/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>24/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -3563,6 +3792,18 @@
                     <c:v>Preço Unitário</c:v>
                   </c:pt>
                   <c:pt idx="12">
+                    <c:v>Preço Unitário</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>Preço Unitário</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>Preço Unitário</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>Preço Unitário</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
                     <c:v>Preço Unitário</c:v>
                   </c:pt>
                 </c:lvl>
@@ -3574,14 +3815,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$6:$AC$6</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$6:$AK$6</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$E$6,GRAFICO!$G$6,GRAFICO!$I$6,GRAFICO!$K$6,GRAFICO!$M$6,GRAFICO!$O$6,GRAFICO!$Q$6,GRAFICO!$S$6,GRAFICO!$U$6,GRAFICO!$W$6,GRAFICO!$Y$6,GRAFICO!$AA$6,GRAFICO!$AC$6)</c:f>
+              <c:f>(GRAFICO!$E$6,GRAFICO!$G$6,GRAFICO!$I$6,GRAFICO!$K$6,GRAFICO!$M$6,GRAFICO!$O$6,GRAFICO!$Q$6,GRAFICO!$S$6,GRAFICO!$U$6,GRAFICO!$W$6,GRAFICO!$Y$6,GRAFICO!$AA$6,GRAFICO!$AC$6,GRAFICO!$AE$6,GRAFICO!$AG$6,GRAFICO!$AI$6,GRAFICO!$AK$6)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                   <c:v>5.0196230136986299E-2</c:v>
                 </c:pt>
@@ -3620,6 +3861,18 @@
                 </c:pt>
                 <c:pt idx="12" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                   <c:v>0.64033217260273978</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>0.68755625753424665</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>0.73555089863013712</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>0.78409593698630153</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>0.83187041917808235</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3669,13 +3922,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$2:$AC$3</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$2:$AK$3</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$E$2:$E$3,GRAFICO!$G$2:$G$3,GRAFICO!$I$2:$I$3,GRAFICO!$K$2:$K$3,GRAFICO!$M$2:$M$3,GRAFICO!$O$2:$O$3,GRAFICO!$Q$2:$Q$3,GRAFICO!$S$2:$S$3,GRAFICO!$U$2:$U$3,GRAFICO!$W$2:$W$3,GRAFICO!$Y$2:$Y$3,GRAFICO!$AA$2:$AA$3,GRAFICO!$AC$2:$AC$3)</c:f>
+              <c:f>(GRAFICO!$E$2:$E$3,GRAFICO!$G$2:$G$3,GRAFICO!$I$2:$I$3,GRAFICO!$K$2:$K$3,GRAFICO!$M$2:$M$3,GRAFICO!$O$2:$O$3,GRAFICO!$Q$2:$Q$3,GRAFICO!$S$2:$S$3,GRAFICO!$U$2:$U$3,GRAFICO!$W$2:$W$3,GRAFICO!$Y$2:$Y$3,GRAFICO!$AA$2:$AA$3,GRAFICO!$AC$2:$AC$3,GRAFICO!$AE$2:$AE$3,GRAFICO!$AG$2:$AG$3,GRAFICO!$AI$2:$AI$3,GRAFICO!$AK$2:$AK$3)</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="17"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>02/05</c:v>
@@ -3715,6 +3968,18 @@
                   </c:pt>
                   <c:pt idx="12">
                     <c:v>20/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>21/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>22/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>23/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>24/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -3755,6 +4020,18 @@
                     <c:v>Preço Unitário</c:v>
                   </c:pt>
                   <c:pt idx="12">
+                    <c:v>Preço Unitário</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>Preço Unitário</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>Preço Unitário</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>Preço Unitário</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
                     <c:v>Preço Unitário</c:v>
                   </c:pt>
                 </c:lvl>
@@ -3766,14 +4043,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>GRAFICO!$B$7:$AC$7</c15:sqref>
+                    <c15:sqref>GRAFICO!$B$7:$AK$7</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(GRAFICO!$E$7,GRAFICO!$G$7,GRAFICO!$I$7,GRAFICO!$K$7,GRAFICO!$M$7,GRAFICO!$O$7,GRAFICO!$Q$7,GRAFICO!$S$7,GRAFICO!$U$7,GRAFICO!$W$7,GRAFICO!$Y$7,GRAFICO!$AA$7,GRAFICO!$AC$7)</c:f>
+              <c:f>(GRAFICO!$E$7,GRAFICO!$G$7,GRAFICO!$I$7,GRAFICO!$K$7,GRAFICO!$M$7,GRAFICO!$O$7,GRAFICO!$Q$7,GRAFICO!$S$7,GRAFICO!$U$7,GRAFICO!$W$7,GRAFICO!$Y$7,GRAFICO!$AA$7,GRAFICO!$AC$7,GRAFICO!$AE$7,GRAFICO!$AG$7,GRAFICO!$AI$7,GRAFICO!$AK$7)</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                   <c:v>4.8875276712328775E-2</c:v>
                 </c:pt>
@@ -3812,6 +4089,18 @@
                 </c:pt>
                 <c:pt idx="12" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
                   <c:v>0.62315977808219181</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>0.67170481643835622</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>0.71837850410958914</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>0.76560258904109602</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>0.81205611780821929</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3828,8 +4117,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-364695552"/>
-        <c:axId val="-364693920"/>
+        <c:axId val="-273370480"/>
+        <c:axId val="-273371568"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -3882,15 +4171,15 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$2:$AC$3</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$2:$AK$3</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$E$2:$E$3,GRAFICO!$G$2:$G$3,GRAFICO!$I$2:$I$3,GRAFICO!$K$2:$K$3,GRAFICO!$M$2:$M$3,GRAFICO!$O$2:$O$3,GRAFICO!$Q$2:$Q$3,GRAFICO!$S$2:$S$3,GRAFICO!$U$2:$U$3,GRAFICO!$W$2:$W$3,GRAFICO!$Y$2:$Y$3,GRAFICO!$AA$2:$AA$3,GRAFICO!$AC$2:$AC$3)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$E$2:$E$3,GRAFICO!$G$2:$G$3,GRAFICO!$I$2:$I$3,GRAFICO!$K$2:$K$3,GRAFICO!$M$2:$M$3,GRAFICO!$O$2:$O$3,GRAFICO!$Q$2:$Q$3,GRAFICO!$S$2:$S$3,GRAFICO!$U$2:$U$3,GRAFICO!$W$2:$W$3,GRAFICO!$Y$2:$Y$3,GRAFICO!$AA$2:$AA$3,GRAFICO!$AC$2:$AC$3,GRAFICO!$AE$2:$AE$3,GRAFICO!$AG$2:$AG$3,GRAFICO!$AI$2:$AI$3,GRAFICO!$AK$2:$AK$3)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:multiLvlStrCache>
-                      <c:ptCount val="13"/>
+                      <c:ptCount val="17"/>
                       <c:lvl>
                         <c:pt idx="0">
                           <c:v>02/05</c:v>
@@ -3930,6 +4219,18 @@
                         </c:pt>
                         <c:pt idx="12">
                           <c:v>20/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="13">
+                          <c:v>21/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="14">
+                          <c:v>22/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="15">
+                          <c:v>23/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="16">
+                          <c:v>24/mai</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
@@ -3970,6 +4271,18 @@
                           <c:v>Preço Unitário</c:v>
                         </c:pt>
                         <c:pt idx="12">
+                          <c:v>Preço Unitário</c:v>
+                        </c:pt>
+                        <c:pt idx="13">
+                          <c:v>Preço Unitário</c:v>
+                        </c:pt>
+                        <c:pt idx="14">
+                          <c:v>Preço Unitário</c:v>
+                        </c:pt>
+                        <c:pt idx="15">
+                          <c:v>Preço Unitário</c:v>
+                        </c:pt>
+                        <c:pt idx="16">
                           <c:v>Preço Unitário</c:v>
                         </c:pt>
                       </c:lvl>
@@ -3981,16 +4294,16 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$4:$AC$4</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$4:$AK$4</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$E$4,GRAFICO!$G$4,GRAFICO!$I$4,GRAFICO!$K$4,GRAFICO!$M$4,GRAFICO!$O$4,GRAFICO!$Q$4,GRAFICO!$S$4,GRAFICO!$U$4,GRAFICO!$W$4,GRAFICO!$Y$4,GRAFICO!$AA$4,GRAFICO!$AC$4)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$E$4,GRAFICO!$G$4,GRAFICO!$I$4,GRAFICO!$K$4,GRAFICO!$M$4,GRAFICO!$O$4,GRAFICO!$Q$4,GRAFICO!$S$4,GRAFICO!$U$4,GRAFICO!$W$4,GRAFICO!$Y$4,GRAFICO!$AA$4,GRAFICO!$AC$4,GRAFICO!$AE$4,GRAFICO!$AG$4,GRAFICO!$AI$4,GRAFICO!$AK$4)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>m/d/yyyy</c:formatCode>
-                      <c:ptCount val="13"/>
+                      <c:ptCount val="17"/>
                       <c:pt idx="0" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>1577.93</c:v>
                       </c:pt>
@@ -4029,6 +4342,18 @@
                       </c:pt>
                       <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>1607.3</c:v>
+                      </c:pt>
+                      <c:pt idx="13" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1652.51</c:v>
+                      </c:pt>
+                      <c:pt idx="14" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1635.37</c:v>
+                      </c:pt>
+                      <c:pt idx="15" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1623.38</c:v>
+                      </c:pt>
+                      <c:pt idx="16" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1641.54</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -4042,7 +4367,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>GRAFICO!$A$5</c15:sqref>
@@ -4086,15 +4411,15 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$2:$AC$3</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$2:$AK$3</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$E$2:$E$3,GRAFICO!$G$2:$G$3,GRAFICO!$I$2:$I$3,GRAFICO!$K$2:$K$3,GRAFICO!$M$2:$M$3,GRAFICO!$O$2:$O$3,GRAFICO!$Q$2:$Q$3,GRAFICO!$S$2:$S$3,GRAFICO!$U$2:$U$3,GRAFICO!$W$2:$W$3,GRAFICO!$Y$2:$Y$3,GRAFICO!$AA$2:$AA$3,GRAFICO!$AC$2:$AC$3)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$E$2:$E$3,GRAFICO!$G$2:$G$3,GRAFICO!$I$2:$I$3,GRAFICO!$K$2:$K$3,GRAFICO!$M$2:$M$3,GRAFICO!$O$2:$O$3,GRAFICO!$Q$2:$Q$3,GRAFICO!$S$2:$S$3,GRAFICO!$U$2:$U$3,GRAFICO!$W$2:$W$3,GRAFICO!$Y$2:$Y$3,GRAFICO!$AA$2:$AA$3,GRAFICO!$AC$2:$AC$3,GRAFICO!$AE$2:$AE$3,GRAFICO!$AG$2:$AG$3,GRAFICO!$AI$2:$AI$3,GRAFICO!$AK$2:$AK$3)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:multiLvlStrCache>
-                      <c:ptCount val="13"/>
+                      <c:ptCount val="17"/>
                       <c:lvl>
                         <c:pt idx="0">
                           <c:v>02/05</c:v>
@@ -4134,6 +4459,18 @@
                         </c:pt>
                         <c:pt idx="12">
                           <c:v>20/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="13">
+                          <c:v>21/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="14">
+                          <c:v>22/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="15">
+                          <c:v>23/mai</c:v>
+                        </c:pt>
+                        <c:pt idx="16">
+                          <c:v>24/mai</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
@@ -4174,6 +4511,18 @@
                           <c:v>Preço Unitário</c:v>
                         </c:pt>
                         <c:pt idx="12">
+                          <c:v>Preço Unitário</c:v>
+                        </c:pt>
+                        <c:pt idx="13">
+                          <c:v>Preço Unitário</c:v>
+                        </c:pt>
+                        <c:pt idx="14">
+                          <c:v>Preço Unitário</c:v>
+                        </c:pt>
+                        <c:pt idx="15">
+                          <c:v>Preço Unitário</c:v>
+                        </c:pt>
+                        <c:pt idx="16">
                           <c:v>Preço Unitário</c:v>
                         </c:pt>
                       </c:lvl>
@@ -4185,16 +4534,16 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>GRAFICO!$B$5:$AC$5</c15:sqref>
+                          <c15:sqref>GRAFICO!$B$5:$AK$5</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(GRAFICO!$E$5,GRAFICO!$G$5,GRAFICO!$I$5,GRAFICO!$K$5,GRAFICO!$M$5,GRAFICO!$O$5,GRAFICO!$Q$5,GRAFICO!$S$5,GRAFICO!$U$5,GRAFICO!$W$5,GRAFICO!$Y$5,GRAFICO!$AA$5,GRAFICO!$AC$5)</c15:sqref>
+                          <c15:sqref>(GRAFICO!$E$5,GRAFICO!$G$5,GRAFICO!$I$5,GRAFICO!$K$5,GRAFICO!$M$5,GRAFICO!$O$5,GRAFICO!$Q$5,GRAFICO!$S$5,GRAFICO!$U$5,GRAFICO!$W$5,GRAFICO!$Y$5,GRAFICO!$AA$5,GRAFICO!$AC$5,GRAFICO!$AE$5,GRAFICO!$AG$5,GRAFICO!$AI$5,GRAFICO!$AK$5)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>m/d/yyyy</c:formatCode>
-                      <c:ptCount val="13"/>
+                      <c:ptCount val="17"/>
                       <c:pt idx="0" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>1607.16</c:v>
                       </c:pt>
@@ -4233,6 +4582,18 @@
                       </c:pt>
                       <c:pt idx="12" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
                         <c:v>1637.01</c:v>
+                      </c:pt>
+                      <c:pt idx="13" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1622.51</c:v>
+                      </c:pt>
+                      <c:pt idx="14" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1665.62</c:v>
+                      </c:pt>
+                      <c:pt idx="15" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1653.38</c:v>
+                      </c:pt>
+                      <c:pt idx="16" formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)">
+                        <c:v>1671.89</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -4244,7 +4605,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-364695552"/>
+        <c:axId val="-273370480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4287,7 +4648,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-364693920"/>
+        <c:crossAx val="-273371568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4295,7 +4656,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-364693920"/>
+        <c:axId val="-273371568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4346,7 +4707,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-364695552"/>
+        <c:crossAx val="-273370480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4360,6 +4721,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6743,6 +7105,7 @@
       <sheetName val="210519"/>
       <sheetName val="220519"/>
       <sheetName val="230519"/>
+      <sheetName val="240519"/>
       <sheetName val="COMPARAÇÃO DIA A DIA"/>
       <sheetName val="TESOURO IPCA"/>
       <sheetName val="TESOURO IPCA JUROS SEMESTRAIS"/>
@@ -6763,26 +7126,27 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="21" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6808,6 +7172,7 @@
       <sheetName val="210519"/>
       <sheetName val="220519"/>
       <sheetName val="230519"/>
+      <sheetName val="240519"/>
       <sheetName val="COMPARAÇÃO DIA A DIA"/>
       <sheetName val="TESOURO IPCA"/>
       <sheetName val="TESOURO IPCA JUROS SEMESTRAIS"/>
@@ -6824,34 +7189,29 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17">
-        <row r="5">
-          <cell r="R5">
-            <v>2614.1</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -7236,8 +7596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:DP11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AI5" sqref="AI5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="AJ5" sqref="AJ5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7277,7 +7637,9 @@
     <col min="33" max="33" width="14.42578125" style="48" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="28.85546875" style="48" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="14.42578125" style="48" bestFit="1" customWidth="1"/>
-    <col min="36" max="120" width="9.140625" style="48"/>
+    <col min="36" max="36" width="28.85546875" style="48" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14.42578125" style="48" bestFit="1" customWidth="1"/>
+    <col min="38" max="120" width="9.140625" style="48"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:120" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7383,8 +7745,12 @@
       <c r="AI2" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="AJ2" s="47"/>
-      <c r="AK2" s="47"/>
+      <c r="AJ2" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="AK2" s="22" t="s">
+        <v>12</v>
+      </c>
       <c r="AL2" s="47"/>
       <c r="AM2" s="47"/>
       <c r="AN2" s="47"/>
@@ -7570,8 +7936,12 @@
       <c r="AI3" s="29">
         <v>43608</v>
       </c>
-      <c r="AJ3" s="47"/>
-      <c r="AK3" s="47"/>
+      <c r="AJ3" s="28">
+        <v>43609</v>
+      </c>
+      <c r="AK3" s="29">
+        <v>43609</v>
+      </c>
       <c r="AL3" s="47"/>
       <c r="AM3" s="47"/>
       <c r="AN3" s="47"/>
@@ -7762,8 +8132,12 @@
       <c r="AI4" s="40">
         <v>1623.38</v>
       </c>
-      <c r="AJ4" s="47"/>
-      <c r="AK4" s="47"/>
+      <c r="AJ4" s="39">
+        <v>4.34</v>
+      </c>
+      <c r="AK4" s="40">
+        <v>1641.54</v>
+      </c>
       <c r="AL4" s="47"/>
       <c r="AM4" s="47"/>
       <c r="AN4" s="47"/>
@@ -7954,6 +8328,12 @@
       <c r="AI5" s="18">
         <v>1653.38</v>
       </c>
+      <c r="AJ5" s="51">
+        <v>4.22</v>
+      </c>
+      <c r="AK5" s="52">
+        <v>1671.89</v>
+      </c>
     </row>
     <row r="6" spans="1:120" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="46" t="s">
@@ -8094,6 +8474,14 @@
         <f t="shared" ref="AI6:AI7" si="26">(((AH4/365)*$B$7)/100)+AG6</f>
         <v>0.78409593698630153</v>
       </c>
+      <c r="AJ6" s="56">
+        <f>$B$6/AK4</f>
+        <v>0.24524172175943709</v>
+      </c>
+      <c r="AK6" s="54">
+        <f t="shared" ref="AK6:AK7" si="27">(((AJ4/365)*$B$7)/100)+AI6</f>
+        <v>0.83187041917808235</v>
+      </c>
     </row>
     <row r="7" spans="1:120" x14ac:dyDescent="0.25">
       <c r="A7" s="46" t="s">
@@ -8123,7 +8511,7 @@
         <v>9.7530394520547958E-2</v>
       </c>
       <c r="H7" s="56">
-        <f t="shared" ref="H7" si="27">$B$6/I5</f>
+        <f t="shared" ref="H7" si="28">$B$6/I5</f>
         <v>0.24867137929272118</v>
       </c>
       <c r="I7" s="54">
@@ -8131,7 +8519,7 @@
         <v>0.14596535342465755</v>
       </c>
       <c r="J7" s="56">
-        <f t="shared" ref="J7" si="28">$B$6/K5</f>
+        <f t="shared" ref="J7" si="29">$B$6/K5</f>
         <v>0.24781873222465564</v>
       </c>
       <c r="K7" s="54">
@@ -8139,7 +8527,7 @@
         <v>0.19418015342465755</v>
       </c>
       <c r="L7" s="56">
-        <f t="shared" ref="L7" si="29">$B$6/M5</f>
+        <f t="shared" ref="L7" si="30">$B$6/M5</f>
         <v>0.2473482365854324</v>
       </c>
       <c r="M7" s="54">
@@ -8147,7 +8535,7 @@
         <v>0.24228487397260276</v>
       </c>
       <c r="N7" s="56">
-        <f t="shared" ref="N7" si="30">$B$6/O5</f>
+        <f t="shared" ref="N7" si="31">$B$6/O5</f>
         <v>0.24725556664045298</v>
       </c>
       <c r="O7" s="54">
@@ -8155,7 +8543,7 @@
         <v>0.29038959452054797</v>
       </c>
       <c r="P7" s="56">
-        <f t="shared" ref="P7" si="31">$B$6/Q5</f>
+        <f t="shared" ref="P7" si="32">$B$6/Q5</f>
         <v>0.24527160486979319</v>
       </c>
       <c r="Q7" s="54">
@@ -8163,7 +8551,7 @@
         <v>0.3379439178082192</v>
       </c>
       <c r="R7" s="56">
-        <f t="shared" ref="R7" si="32">$B$6/S5</f>
+        <f t="shared" ref="R7" si="33">$B$6/S5</f>
         <v>0.24443613706365483</v>
       </c>
       <c r="S7" s="54">
@@ -8171,7 +8559,7 @@
         <v>0.38527808219178084</v>
       </c>
       <c r="T7" s="56">
-        <f t="shared" ref="T7" si="33">$B$6/U5</f>
+        <f t="shared" ref="T7" si="34">$B$6/U5</f>
         <v>0.24584827750825125</v>
       </c>
       <c r="U7" s="54">
@@ -8179,7 +8567,7 @@
         <v>0.43305256438356166</v>
       </c>
       <c r="V7" s="56">
-        <f t="shared" ref="V7" si="34">$B$6/W5</f>
+        <f t="shared" ref="V7" si="35">$B$6/W5</f>
         <v>0.24428484495287314</v>
       </c>
       <c r="W7" s="54">
@@ -8187,7 +8575,7 @@
         <v>0.48038672876712329</v>
       </c>
       <c r="X7" s="56">
-        <f t="shared" ref="X7" si="35">$B$6/Y5</f>
+        <f t="shared" ref="X7" si="36">$B$6/Y5</f>
         <v>0.2442211210488876</v>
       </c>
       <c r="Y7" s="54">
@@ -8195,7 +8583,7 @@
         <v>0.52772089315068493</v>
       </c>
       <c r="Z7" s="56">
-        <f t="shared" ref="Z7" si="36">$B$6/AA5</f>
+        <f t="shared" ref="Z7" si="37">$B$6/AA5</f>
         <v>0.24485986006750585</v>
       </c>
       <c r="AA7" s="54">
@@ -8203,7 +8591,7 @@
         <v>0.57527521643835622</v>
       </c>
       <c r="AB7" s="56">
-        <f t="shared" ref="AB7" si="37">$B$6/AC5</f>
+        <f t="shared" ref="AB7" si="38">$B$6/AC5</f>
         <v>0.24592036452861396</v>
       </c>
       <c r="AC7" s="54">
@@ -8211,7 +8599,7 @@
         <v>0.62315977808219181</v>
       </c>
       <c r="AD7" s="56">
-        <f t="shared" ref="AD7" si="38">$B$6/AE5</f>
+        <f t="shared" ref="AD7" si="39">$B$6/AE5</f>
         <v>0.248118098462867</v>
       </c>
       <c r="AE7" s="54">
@@ -8233,6 +8621,14 @@
       <c r="AI7" s="54">
         <f t="shared" si="26"/>
         <v>0.76560258904109602</v>
+      </c>
+      <c r="AJ7" s="56">
+        <f>$B$6/AK5</f>
+        <v>0.24078982225923135</v>
+      </c>
+      <c r="AK7" s="54">
+        <f t="shared" si="27"/>
+        <v>0.81205611780821929</v>
       </c>
     </row>
     <row r="10" spans="1:120" x14ac:dyDescent="0.25">

</xml_diff>